<commit_message>
items yes/no were included in the analysis
</commit_message>
<xml_diff>
--- a/report/reliability/by-unidade/Faculdade de Direito - FDA.xlsx
+++ b/report/reliability/by-unidade/Faculdade de Direito - FDA.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="51">
   <si>
     <t>Reliability Analysis of all</t>
   </si>
@@ -74,22 +74,25 @@
     <t>med.r</t>
   </si>
   <si>
+    <t>Item8</t>
+  </si>
+  <si>
     <t>Item9</t>
   </si>
   <si>
     <t>Item10</t>
   </si>
   <si>
-    <t>Item12</t>
-  </si>
-  <si>
-    <t>Item13</t>
+    <t>Item14</t>
   </si>
   <si>
     <t>Item15</t>
   </si>
   <si>
     <t>Item16</t>
+  </si>
+  <si>
+    <t>Item17</t>
   </si>
   <si>
     <t>Item18</t>
@@ -4128,31 +4131,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="31">
-        <v>0.7811376561541883</v>
+        <v>0.7747770444096332</v>
       </c>
       <c r="B6" t="n" s="32">
-        <v>0.8042661325302204</v>
+        <v>0.7960197620668606</v>
       </c>
       <c r="C6" t="n" s="33">
-        <v>0.9079048931942684</v>
+        <v>0.9077708263697879</v>
       </c>
       <c r="D6" t="n" s="34">
-        <v>0.2550737801856373</v>
+        <v>0.2308800794888843</v>
       </c>
       <c r="E6" t="n" s="35">
-        <v>4.108977883729784</v>
+        <v>3.9024356973629026</v>
       </c>
       <c r="F6" t="n" s="36">
-        <v>0.030901113842690467</v>
+        <v>0.029541406326582094</v>
       </c>
       <c r="G6" t="n" s="37">
-        <v>3.006734006734007</v>
+        <v>2.306138306138306</v>
       </c>
       <c r="H6" t="n" s="38">
-        <v>0.7923311539694512</v>
+        <v>0.7147065368963383</v>
       </c>
       <c r="I6" t="n" s="39">
-        <v>0.19224678870309964</v>
+        <v>0.1786728486529099</v>
       </c>
     </row>
     <row r="7">
@@ -4202,28 +4205,28 @@
         <v>18</v>
       </c>
       <c r="B11" t="n" s="58">
-        <v>0.7658097628366335</v>
+        <v>0.7789595052065731</v>
       </c>
       <c r="C11" t="n" s="59">
-        <v>0.7795255201929654</v>
+        <v>0.7993446983486694</v>
       </c>
       <c r="D11" t="n" s="60">
-        <v>0.8891509159042734</v>
+        <v>0.9088047785818625</v>
       </c>
       <c r="E11" t="n" s="61">
-        <v>0.24324105952596792</v>
+        <v>0.24923379433179585</v>
       </c>
       <c r="F11" t="n" s="62">
-        <v>3.5356723411944433</v>
+        <v>3.9836709609480154</v>
       </c>
       <c r="G11" t="n" s="63">
-        <v>0.033134261749835005</v>
+        <v>0.029832117402365084</v>
       </c>
       <c r="H11" t="n" s="64">
-        <v>0.041515258996651386</v>
+        <v>0.060860271019174184</v>
       </c>
       <c r="I11" t="n" s="65">
-        <v>0.18621948183595435</v>
+        <v>0.19224678870309964</v>
       </c>
     </row>
     <row r="12">
@@ -4231,28 +4234,28 @@
         <v>19</v>
       </c>
       <c r="B12" t="n" s="58">
-        <v>0.7699594746641973</v>
+        <v>0.7628878961200659</v>
       </c>
       <c r="C12" t="n" s="59">
-        <v>0.7857296434497623</v>
+        <v>0.7790810070313358</v>
       </c>
       <c r="D12" t="n" s="60">
-        <v>0.8992985546337158</v>
+        <v>0.8993197474414234</v>
       </c>
       <c r="E12" t="n" s="61">
-        <v>0.25001710376847414</v>
+        <v>0.22713010711864975</v>
       </c>
       <c r="F12" t="n" s="62">
-        <v>3.667001147989127</v>
+        <v>3.526546072667655</v>
       </c>
       <c r="G12" t="n" s="63">
-        <v>0.03238199995917217</v>
+        <v>0.031215674331133196</v>
       </c>
       <c r="H12" t="n" s="64">
-        <v>0.04341411743977191</v>
+        <v>0.06250710673152261</v>
       </c>
       <c r="I12" t="n" s="65">
-        <v>0.18621948183595435</v>
+        <v>0.17186792033315917</v>
       </c>
     </row>
     <row r="13">
@@ -4260,28 +4263,28 @@
         <v>20</v>
       </c>
       <c r="B13" t="n" s="58">
-        <v>0.7683569697691971</v>
+        <v>0.7677075036850112</v>
       </c>
       <c r="C13" t="n" s="59">
-        <v>0.7818552493721105</v>
+        <v>0.7839282588804578</v>
       </c>
       <c r="D13" t="n" s="60">
-        <v>0.8901589189596169</v>
+        <v>0.9028767130555284</v>
       </c>
       <c r="E13" t="n" s="61">
-        <v>0.24575456543885865</v>
+        <v>0.2321519714498712</v>
       </c>
       <c r="F13" t="n" s="62">
-        <v>3.584112141693458</v>
+        <v>3.6280924790009834</v>
       </c>
       <c r="G13" t="n" s="63">
-        <v>0.0327647155766314</v>
+        <v>0.030405323812863545</v>
       </c>
       <c r="H13" t="n" s="64">
-        <v>0.042426193274487586</v>
+        <v>0.063746222060938</v>
       </c>
       <c r="I13" t="n" s="65">
-        <v>0.19593580758082565</v>
+        <v>0.1649040980297498</v>
       </c>
     </row>
     <row r="14">
@@ -4289,28 +4292,28 @@
         <v>21</v>
       </c>
       <c r="B14" t="n" s="58">
-        <v>0.7748311859813796</v>
+        <v>0.7579881289682129</v>
       </c>
       <c r="C14" t="n" s="59">
-        <v>0.7932486436435348</v>
+        <v>0.7693792023554421</v>
       </c>
       <c r="D14" t="n" s="60">
-        <v>0.898715105676986</v>
+        <v>0.8871734375602608</v>
       </c>
       <c r="E14" t="n" s="61">
-        <v>0.25859662140229545</v>
+        <v>0.2175336301241691</v>
       </c>
       <c r="F14" t="n" s="62">
-        <v>3.8367276404991237</v>
+        <v>3.3361223715011197</v>
       </c>
       <c r="G14" t="n" s="63">
-        <v>0.031749327977778144</v>
+        <v>0.032433515085561096</v>
       </c>
       <c r="H14" t="n" s="64">
-        <v>0.04327218819689618</v>
+        <v>0.050314005941136546</v>
       </c>
       <c r="I14" t="n" s="65">
-        <v>0.19773617988402772</v>
+        <v>0.1776076099399131</v>
       </c>
     </row>
     <row r="15">
@@ -4318,28 +4321,28 @@
         <v>22</v>
       </c>
       <c r="B15" t="n" s="58">
-        <v>0.7392167779651636</v>
+        <v>0.7230661238242313</v>
       </c>
       <c r="C15" t="n" s="59">
-        <v>0.7814551724458865</v>
+        <v>0.7622841254998607</v>
       </c>
       <c r="D15" t="n" s="60">
-        <v>0.8729548325735723</v>
+        <v>0.8839257642374267</v>
       </c>
       <c r="E15" t="n" s="61">
-        <v>0.24532031439535296</v>
+        <v>0.21087429184610976</v>
       </c>
       <c r="F15" t="n" s="62">
-        <v>3.5757202821576333</v>
+        <v>3.206702653336744</v>
       </c>
       <c r="G15" t="n" s="63">
-        <v>0.03849375672040325</v>
+        <v>0.03822333976247019</v>
       </c>
       <c r="H15" t="n" s="64">
-        <v>0.04027726901540908</v>
+        <v>0.04998499739662411</v>
       </c>
       <c r="I15" t="n" s="65">
-        <v>0.18385388666170893</v>
+        <v>0.1618230409010712</v>
       </c>
     </row>
     <row r="16">
@@ -4347,28 +4350,28 @@
         <v>23</v>
       </c>
       <c r="B16" t="n" s="58">
-        <v>0.7381208629768411</v>
+        <v>0.7231955914995614</v>
       </c>
       <c r="C16" t="n" s="59">
-        <v>0.7798863590100011</v>
+        <v>0.7617645949006973</v>
       </c>
       <c r="D16" t="n" s="60">
-        <v>0.8724738387762536</v>
+        <v>0.8864326308630778</v>
       </c>
       <c r="E16" t="n" s="61">
-        <v>0.24362796805474665</v>
+        <v>0.21039794877016052</v>
       </c>
       <c r="F16" t="n" s="62">
-        <v>3.543107803325264</v>
+        <v>3.1975289087832017</v>
       </c>
       <c r="G16" t="n" s="63">
-        <v>0.03887650967484679</v>
+        <v>0.038443123323745915</v>
       </c>
       <c r="H16" t="n" s="64">
-        <v>0.04053963599055971</v>
+        <v>0.050613907289312345</v>
       </c>
       <c r="I16" t="n" s="65">
-        <v>0.18299260948072463</v>
+        <v>0.1645494079638074</v>
       </c>
     </row>
     <row r="17">
@@ -4376,28 +4379,28 @@
         <v>24</v>
       </c>
       <c r="B17" t="n" s="58">
-        <v>0.7798448996741202</v>
+        <v>0.7748283043446783</v>
       </c>
       <c r="C17" t="n" s="59">
-        <v>0.8093395543183953</v>
+        <v>0.8013729562148169</v>
       </c>
       <c r="D17" t="n" s="60">
-        <v>0.8971559513642836</v>
+        <v>0.9035600965149932</v>
       </c>
       <c r="E17" t="n" s="61">
-        <v>0.2784484667050163</v>
+        <v>0.25161656249070763</v>
       </c>
       <c r="F17" t="n" s="62">
-        <v>4.244926373821444</v>
+        <v>4.034561160168648</v>
       </c>
       <c r="G17" t="n" s="63">
-        <v>0.030845130396610326</v>
+        <v>0.030052049433717486</v>
       </c>
       <c r="H17" t="n" s="64">
-        <v>0.03957883161028481</v>
+        <v>0.05385179959156182</v>
       </c>
       <c r="I17" t="n" s="65">
-        <v>0.22090833933996992</v>
+        <v>0.1968359937324267</v>
       </c>
     </row>
     <row r="18">
@@ -4405,28 +4408,28 @@
         <v>25</v>
       </c>
       <c r="B18" t="n" s="58">
-        <v>0.7798294162546576</v>
+        <v>0.769634703196347</v>
       </c>
       <c r="C18" t="n" s="59">
-        <v>0.8035363119209845</v>
+        <v>0.7904919244774175</v>
       </c>
       <c r="D18" t="n" s="60">
-        <v>0.891718106930177</v>
+        <v>0.8958587113317913</v>
       </c>
       <c r="E18" t="n" s="61">
-        <v>0.271040381750503</v>
+        <v>0.23921037229263736</v>
       </c>
       <c r="F18" t="n" s="62">
-        <v>4.089999122880206</v>
+        <v>3.7730857032869465</v>
       </c>
       <c r="G18" t="n" s="63">
-        <v>0.03033562784973592</v>
+        <v>0.029244022757729547</v>
       </c>
       <c r="H18" t="n" s="64">
-        <v>0.041595502279877225</v>
+        <v>0.05644373350934114</v>
       </c>
       <c r="I18" t="n" s="65">
-        <v>0.21865658905184612</v>
+        <v>0.19079503327286834</v>
       </c>
     </row>
     <row r="19">
@@ -4434,28 +4437,28 @@
         <v>26</v>
       </c>
       <c r="B19" t="n" s="58">
-        <v>0.7729731315264579</v>
+        <v>0.7728230597031442</v>
       </c>
       <c r="C19" t="n" s="59">
-        <v>0.797311861893119</v>
+        <v>0.788777009560541</v>
       </c>
       <c r="D19" t="n" s="60">
-        <v>0.9035717752551886</v>
+        <v>0.9010595150114621</v>
       </c>
       <c r="E19" t="n" s="61">
-        <v>0.26341034269786384</v>
+        <v>0.2373365997714637</v>
       </c>
       <c r="F19" t="n" s="62">
-        <v>3.9336878287010655</v>
+        <v>3.7343331231105803</v>
       </c>
       <c r="G19" t="n" s="63">
-        <v>0.03184394770128798</v>
+        <v>0.02837948489837348</v>
       </c>
       <c r="H19" t="n" s="64">
-        <v>0.04446456364876602</v>
+        <v>0.05876205616098885</v>
       </c>
       <c r="I19" t="n" s="65">
-        <v>0.18621948183595435</v>
+        <v>0.19224678870309964</v>
       </c>
     </row>
     <row r="20">
@@ -4463,28 +4466,28 @@
         <v>27</v>
       </c>
       <c r="B20" t="n" s="58">
-        <v>0.7673312604316697</v>
+        <v>0.7650445641318869</v>
       </c>
       <c r="C20" t="n" s="59">
-        <v>0.7903260764632978</v>
+        <v>0.7876446205887192</v>
       </c>
       <c r="D20" t="n" s="60">
-        <v>0.8970161283509127</v>
+        <v>0.9039278627316366</v>
       </c>
       <c r="E20" t="n" s="61">
-        <v>0.2552123431760727</v>
+        <v>0.23611093096897587</v>
       </c>
       <c r="F20" t="n" s="62">
-        <v>3.7693102849051003</v>
+        <v>3.7090872045357663</v>
       </c>
       <c r="G20" t="n" s="63">
-        <v>0.032282820987762056</v>
+        <v>0.030072660848048806</v>
       </c>
       <c r="H20" t="n" s="64">
-        <v>0.045814533621642985</v>
+        <v>0.06264257330206052</v>
       </c>
       <c r="I20" t="n" s="65">
-        <v>0.19593580758082565</v>
+        <v>0.17186792033315917</v>
       </c>
     </row>
     <row r="21">
@@ -4492,28 +4495,28 @@
         <v>28</v>
       </c>
       <c r="B21" t="n" s="58">
-        <v>0.7604852608547623</v>
+        <v>0.7611182850185308</v>
       </c>
       <c r="C21" t="n" s="59">
-        <v>0.7888029821161407</v>
+        <v>0.7818909166939616</v>
       </c>
       <c r="D21" t="n" s="60">
-        <v>0.8889268049753485</v>
+        <v>0.8985816643050275</v>
       </c>
       <c r="E21" t="n" s="61">
-        <v>0.2534738242287807</v>
+        <v>0.23002204516695943</v>
       </c>
       <c r="F21" t="n" s="62">
-        <v>3.734915341228522</v>
+        <v>3.5848617803636205</v>
       </c>
       <c r="G21" t="n" s="63">
-        <v>0.03383220080005177</v>
+        <v>0.030337373875587575</v>
       </c>
       <c r="H21" t="n" s="64">
-        <v>0.04337725610503386</v>
+        <v>0.0635896828899669</v>
       </c>
       <c r="I21" t="n" s="65">
-        <v>0.19593580758082565</v>
+        <v>0.1786728486529099</v>
       </c>
     </row>
     <row r="22">
@@ -4521,33 +4524,57 @@
         <v>29</v>
       </c>
       <c r="B22" t="n" s="58">
-        <v>0.7622333722042974</v>
+        <v>0.752236814675839</v>
       </c>
       <c r="C22" t="n" s="59">
-        <v>0.7881576781886123</v>
+        <v>0.7801524351197503</v>
       </c>
       <c r="D22" t="n" s="60">
-        <v>0.8888471816719115</v>
+        <v>0.8896426218293768</v>
       </c>
       <c r="E22" t="n" s="61">
-        <v>0.25274237108371556</v>
+        <v>0.22822664398643844</v>
       </c>
       <c r="F22" t="n" s="62">
-        <v>3.720492069050973</v>
+        <v>3.5486062151504703</v>
       </c>
       <c r="G22" t="n" s="63">
-        <v>0.033394408727202056</v>
+        <v>0.03219830845729027</v>
       </c>
       <c r="H22" t="n" s="64">
-        <v>0.0440557204251918</v>
+        <v>0.0607153516643284</v>
       </c>
       <c r="I22" t="n" s="65">
-        <v>0.19593580758082565</v>
+        <v>0.17328784911209832</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>1</v>
+      <c r="A23" t="s" s="53">
+        <v>30</v>
+      </c>
+      <c r="B23" t="n" s="58">
+        <v>0.7555099136590848</v>
+      </c>
+      <c r="C23" t="n" s="59">
+        <v>0.7833991786963367</v>
+      </c>
+      <c r="D23" t="n" s="60">
+        <v>0.8892012057852741</v>
+      </c>
+      <c r="E23" t="n" s="61">
+        <v>0.23159613503755727</v>
+      </c>
+      <c r="F23" t="n" s="62">
+        <v>3.616787664890941</v>
+      </c>
+      <c r="G23" t="n" s="63">
+        <v>0.03161033209676899</v>
+      </c>
+      <c r="H23" t="n" s="64">
+        <v>0.06018644281467542</v>
+      </c>
+      <c r="I23" t="n" s="65">
+        <v>0.17328784911209832</v>
       </c>
     </row>
     <row r="24">
@@ -4556,458 +4583,437 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="69">
-        <v>30</v>
+      <c r="A25" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26"/>
-      <c r="B26" t="s" s="83">
+      <c r="A26" t="s" s="69">
         <v>31</v>
       </c>
-      <c r="C26" t="s" s="83">
+    </row>
+    <row r="27">
+      <c r="A27"/>
+      <c r="B27" t="s" s="83">
         <v>32</v>
       </c>
-      <c r="D26" t="s" s="83">
+      <c r="C27" t="s" s="83">
         <v>33</v>
       </c>
-      <c r="E26" t="s" s="83">
+      <c r="D27" t="s" s="83">
         <v>34</v>
       </c>
-      <c r="F26" t="s" s="83">
+      <c r="E27" t="s" s="83">
         <v>35</v>
       </c>
-      <c r="G26" t="s" s="83">
+      <c r="F27" t="s" s="83">
+        <v>36</v>
+      </c>
+      <c r="G27" t="s" s="83">
         <v>9</v>
       </c>
-      <c r="H26" t="s" s="83">
+      <c r="H27" t="s" s="83">
         <v>10</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="79">
-        <v>18</v>
-      </c>
-      <c r="B27" t="n" s="84">
-        <v>99.0</v>
-      </c>
-      <c r="C27" t="n" s="85">
-        <v>0.5612206374953863</v>
-      </c>
-      <c r="D27" t="n" s="86">
-        <v>0.6594630766611417</v>
-      </c>
-      <c r="E27" t="n" s="87">
-        <v>0.6412700870499489</v>
-      </c>
-      <c r="F27" t="n" s="88">
-        <v>0.4967726259340483</v>
-      </c>
-      <c r="G27" t="n" s="89">
-        <v>3.888888888888889</v>
-      </c>
-      <c r="H27" t="n" s="90">
-        <v>0.8316309141225229</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="79">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C28" t="n" s="85">
-        <v>0.48753709896563063</v>
+        <v>0.20740155132644558</v>
       </c>
       <c r="D28" t="n" s="86">
-        <v>0.6043157254414473</v>
+        <v>0.36553775889415246</v>
       </c>
       <c r="E28" t="n" s="87">
-        <v>0.5594679328677249</v>
+        <v>0.2934713469573362</v>
       </c>
       <c r="F28" t="n" s="88">
-        <v>0.4096761312474632</v>
+        <v>0.19701538621861703</v>
       </c>
       <c r="G28" t="n" s="89">
-        <v>4.474747474747475</v>
+        <v>0.98989898989899</v>
       </c>
       <c r="H28" t="n" s="90">
-        <v>0.9073783085152335</v>
+        <v>0.10050378152592121</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="79">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C29" t="n" s="85">
-        <v>0.5275379790963006</v>
+        <v>0.48832954512153554</v>
       </c>
       <c r="D29" t="n" s="86">
-        <v>0.6390067176985718</v>
+        <v>0.5739071884371174</v>
       </c>
       <c r="E29" t="n" s="87">
-        <v>0.6173961090417365</v>
+        <v>0.5311841107450963</v>
       </c>
       <c r="F29" t="n" s="88">
-        <v>0.4628190833076534</v>
+        <v>0.415666705469007</v>
       </c>
       <c r="G29" t="n" s="89">
-        <v>3.9292929292929295</v>
+        <v>3.888888888888889</v>
       </c>
       <c r="H29" t="n" s="90">
-        <v>0.7986279720912847</v>
+        <v>0.8316309141225229</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="79">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C30" t="n" s="85">
-        <v>0.41569684920966576</v>
+        <v>0.41146114003254075</v>
       </c>
       <c r="D30" t="n" s="86">
-        <v>0.5344906689165937</v>
+        <v>0.5265665345521655</v>
       </c>
       <c r="E30" t="n" s="87">
-        <v>0.4914795514130755</v>
+        <v>0.4704125436048257</v>
       </c>
       <c r="F30" t="n" s="88">
-        <v>0.33103263759308166</v>
+        <v>0.3255416518087932</v>
       </c>
       <c r="G30" t="n" s="89">
-        <v>4.515151515151516</v>
+        <v>4.474747474747475</v>
       </c>
       <c r="H30" t="n" s="90">
-        <v>0.9187795405622853</v>
+        <v>0.9073783085152335</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="79">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C31" t="n" s="85">
-        <v>0.7574575434821654</v>
+        <v>0.7325070961532397</v>
       </c>
       <c r="D31" t="n" s="86">
-        <v>0.6425409028302892</v>
+        <v>0.6643722958049441</v>
       </c>
       <c r="E31" t="n" s="87">
-        <v>0.6661741812183487</v>
+        <v>0.6911510532655667</v>
       </c>
       <c r="F31" t="n" s="88">
-        <v>0.6284173295093756</v>
+        <v>0.7059010063622054</v>
       </c>
       <c r="G31" t="n" s="89">
-        <v>2.1818181818181817</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="H31" t="n" s="90">
-        <v>2.1869913932980913</v>
+        <v>0.5023137559951615</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="79">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C32" t="n" s="85">
-        <v>0.768379029197882</v>
+        <v>0.7966333615798016</v>
       </c>
       <c r="D32" t="n" s="86">
-        <v>0.6563141921847669</v>
+        <v>0.7271492662150024</v>
       </c>
       <c r="E32" t="n" s="87">
-        <v>0.6806108283070071</v>
+        <v>0.7590995164143669</v>
       </c>
       <c r="F32" t="n" s="88">
-        <v>0.6379662336618831</v>
+        <v>0.6804270078163962</v>
       </c>
       <c r="G32" t="n" s="89">
-        <v>2.212121212121212</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="H32" t="n" s="90">
-        <v>2.264512053909309</v>
+        <v>2.1869913932980913</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="79">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C33" t="n" s="85">
-        <v>0.42721885197697673</v>
+        <v>0.8014007393402219</v>
       </c>
       <c r="D33" t="n" s="86">
-        <v>0.372924916674211</v>
+        <v>0.7316397086486633</v>
       </c>
       <c r="E33" t="n" s="87">
-        <v>0.32771379445377297</v>
+        <v>0.7602369625518662</v>
       </c>
       <c r="F33" t="n" s="88">
-        <v>0.28556480730596717</v>
+        <v>0.6819398933575034</v>
       </c>
       <c r="G33" t="n" s="89">
-        <v>2.4646464646464645</v>
+        <v>2.212121212121212</v>
       </c>
       <c r="H33" t="n" s="90">
-        <v>1.5004294032527945</v>
+        <v>2.264512053909309</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="79">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C34" t="n" s="85">
-        <v>0.4771636694138359</v>
+        <v>0.30182565153998564</v>
       </c>
       <c r="D34" t="n" s="86">
-        <v>0.4332161792797769</v>
+        <v>0.3430756222733313</v>
       </c>
       <c r="E34" t="n" s="87">
-        <v>0.3980022611882636</v>
+        <v>0.3025540216180086</v>
       </c>
       <c r="F34" t="n" s="88">
-        <v>0.31501984162634705</v>
+        <v>0.2649977096176945</v>
       </c>
       <c r="G34" t="n" s="89">
-        <v>2.494949494949495</v>
+        <v>0.8383838383838383</v>
       </c>
       <c r="H34" t="n" s="90">
-        <v>1.7634251074735523</v>
+        <v>0.3699716124540519</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="79">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C35" t="n" s="85">
-        <v>0.5062994812973695</v>
+        <v>0.45669118324800984</v>
       </c>
       <c r="D35" t="n" s="86">
-        <v>0.4953138321871086</v>
+        <v>0.4600276379911413</v>
       </c>
       <c r="E35" t="n" s="87">
-        <v>0.4319983443010401</v>
+        <v>0.4378389875667666</v>
       </c>
       <c r="F35" t="n" s="88">
-        <v>0.3610610299495395</v>
+        <v>0.3149406955390899</v>
       </c>
       <c r="G35" t="n" s="89">
-        <v>2.080808080808081</v>
+        <v>2.4646464646464645</v>
       </c>
       <c r="H35" t="n" s="90">
-        <v>1.6392928271041933</v>
+        <v>1.5004294032527945</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="79">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C36" t="n" s="85">
-        <v>0.5177434337696255</v>
+        <v>0.48141499848832164</v>
       </c>
       <c r="D36" t="n" s="86">
-        <v>0.5620338745521045</v>
+        <v>0.47769151947685223</v>
       </c>
       <c r="E36" t="n" s="87">
-        <v>0.5147029443738631</v>
+        <v>0.44338242215653306</v>
       </c>
       <c r="F36" t="n" s="88">
-        <v>0.40682592795935374</v>
+        <v>0.3156969489517907</v>
       </c>
       <c r="G36" t="n" s="89">
-        <v>2.727272727272727</v>
+        <v>2.494949494949495</v>
       </c>
       <c r="H36" t="n" s="90">
-        <v>1.3000642199065635</v>
+        <v>1.7634251074735523</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="79">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C37" t="n" s="85">
-        <v>0.5829671317630193</v>
+        <v>0.5153044375721368</v>
       </c>
       <c r="D37" t="n" s="86">
-        <v>0.5761829431763896</v>
+        <v>0.48924578672286684</v>
       </c>
       <c r="E37" t="n" s="87">
-        <v>0.5526289122556934</v>
+        <v>0.42622409964434327</v>
       </c>
       <c r="F37" t="n" s="88">
-        <v>0.48571852892971307</v>
+        <v>0.3677080231361852</v>
       </c>
       <c r="G37" t="n" s="89">
-        <v>2.7373737373737375</v>
+        <v>2.080808080808081</v>
       </c>
       <c r="H37" t="n" s="90">
-        <v>1.2501906677918566</v>
+        <v>1.6392928271041933</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="79">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" t="n" s="84">
         <v>99.0</v>
       </c>
       <c r="C38" t="n" s="85">
-        <v>0.5664974004252391</v>
+        <v>0.5080902056681977</v>
       </c>
       <c r="D38" t="n" s="86">
-        <v>0.5821359302065822</v>
+        <v>0.5466451540267911</v>
       </c>
       <c r="E38" t="n" s="87">
-        <v>0.557792546815227</v>
+        <v>0.49862497231852765</v>
       </c>
       <c r="F38" t="n" s="88">
-        <v>0.47048222090911346</v>
+        <v>0.39304921283119076</v>
       </c>
       <c r="G38" t="n" s="89">
+        <v>2.727272727272727</v>
+      </c>
+      <c r="H38" t="n" s="90">
+        <v>1.3000642199065635</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="79">
+        <v>29</v>
+      </c>
+      <c r="B39" t="n" s="84">
+        <v>99.0</v>
+      </c>
+      <c r="C39" t="n" s="85">
+        <v>0.5907483883553031</v>
+      </c>
+      <c r="D39" t="n" s="86">
+        <v>0.5635702360811292</v>
+      </c>
+      <c r="E39" t="n" s="87">
+        <v>0.5444693581299221</v>
+      </c>
+      <c r="F39" t="n" s="88">
+        <v>0.4921740082130895</v>
+      </c>
+      <c r="G39" t="n" s="89">
+        <v>2.7373737373737375</v>
+      </c>
+      <c r="H39" t="n" s="90">
+        <v>1.2501906677918566</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="79">
+        <v>30</v>
+      </c>
+      <c r="B40" t="n" s="84">
+        <v>99.0</v>
+      </c>
+      <c r="C40" t="n" s="85">
+        <v>0.5594868430396914</v>
+      </c>
+      <c r="D40" t="n" s="86">
+        <v>0.5318063533677423</v>
+      </c>
+      <c r="E40" t="n" s="87">
+        <v>0.511917899387864</v>
+      </c>
+      <c r="F40" t="n" s="88">
+        <v>0.46000321863834154</v>
+      </c>
+      <c r="G40" t="n" s="89">
         <v>2.3737373737373737</v>
       </c>
-      <c r="H38" t="n" s="90">
+      <c r="H40" t="n" s="90">
         <v>1.208691809150421</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="s">
+    <row r="41">
+      <c r="A41" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="s">
+    <row r="42">
+      <c r="A42" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s" s="94">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42"/>
-      <c r="B42" t="s" s="108">
+    <row r="43">
+      <c r="A43" t="s" s="94">
         <v>37</v>
       </c>
-      <c r="C42" t="s" s="108">
+    </row>
+    <row r="44">
+      <c r="A44"/>
+      <c r="B44" t="s" s="108">
         <v>38</v>
       </c>
-      <c r="D42" t="s" s="108">
+      <c r="C44" t="s" s="108">
         <v>39</v>
       </c>
-      <c r="E42" t="s" s="108">
+      <c r="D44" t="s" s="108">
         <v>40</v>
       </c>
-      <c r="F42" t="s" s="108">
+      <c r="E44" t="s" s="108">
         <v>41</v>
       </c>
-      <c r="G42" t="s" s="108">
+      <c r="F44" t="s" s="108">
         <v>42</v>
       </c>
-      <c r="H42" t="s" s="108">
+      <c r="G44" t="s" s="108">
         <v>43</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="104">
-        <v>18</v>
-      </c>
-      <c r="B43" t="n" s="109">
-        <v>0.010101010101010102</v>
-      </c>
-      <c r="C43" t="n" s="110">
-        <v>0.010101010101010102</v>
-      </c>
-      <c r="D43" t="n" s="111">
-        <v>0.0</v>
-      </c>
-      <c r="E43" t="n" s="112">
-        <v>0.24242424242424243</v>
-      </c>
-      <c r="F43" t="n" s="113">
-        <v>0.5353535353535354</v>
-      </c>
-      <c r="G43" t="n" s="114">
-        <v>0.20202020202020202</v>
-      </c>
-      <c r="H43" t="n" s="115">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="104">
-        <v>19</v>
-      </c>
-      <c r="B44" t="n" s="109">
-        <v>0.010101010101010102</v>
-      </c>
-      <c r="C44" t="n" s="110">
-        <v>0.0</v>
-      </c>
-      <c r="D44" t="n" s="111">
-        <v>0.0</v>
-      </c>
-      <c r="E44" t="n" s="112">
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="F44" t="n" s="113">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="G44" t="n" s="114">
-        <v>0.696969696969697</v>
-      </c>
-      <c r="H44" t="n" s="115">
-        <v>0.0</v>
+      <c r="H44" t="s" s="108">
+        <v>44</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="104">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B45" t="n" s="109">
-        <v>0.0</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="C45" t="n" s="110">
-        <v>0.020202020202020204</v>
+        <v>0.98989898989899</v>
       </c>
       <c r="D45" t="n" s="111">
-        <v>0.010101010101010102</v>
+        <v>0.0</v>
       </c>
       <c r="E45" t="n" s="112">
-        <v>0.20202020202020202</v>
+        <v>0.0</v>
       </c>
       <c r="F45" t="n" s="113">
-        <v>0.5555555555555556</v>
+        <v>0.0</v>
       </c>
       <c r="G45" t="n" s="114">
-        <v>0.21212121212121213</v>
+        <v>0.0</v>
       </c>
       <c r="H45" t="n" s="115">
         <v>0.0</v>
@@ -5015,25 +5021,25 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="104">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B46" t="n" s="109">
-        <v>0.0</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="C46" t="n" s="110">
         <v>0.010101010101010102</v>
       </c>
       <c r="D46" t="n" s="111">
-        <v>0.020202020202020204</v>
+        <v>0.0</v>
       </c>
       <c r="E46" t="n" s="112">
-        <v>0.1717171717171717</v>
+        <v>0.24242424242424243</v>
       </c>
       <c r="F46" t="n" s="113">
-        <v>0.04040404040404041</v>
+        <v>0.5353535353535354</v>
       </c>
       <c r="G46" t="n" s="114">
-        <v>0.7575757575757576</v>
+        <v>0.20202020202020202</v>
       </c>
       <c r="H46" t="n" s="115">
         <v>0.0</v>
@@ -5041,10 +5047,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="104">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B47" t="n" s="109">
-        <v>0.48484848484848486</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="C47" t="n" s="110">
         <v>0.0</v>
@@ -5053,13 +5059,13 @@
         <v>0.0</v>
       </c>
       <c r="E47" t="n" s="112">
-        <v>0.08080808080808081</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="F47" t="n" s="113">
-        <v>0.23232323232323232</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G47" t="n" s="114">
-        <v>0.20202020202020202</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="H47" t="n" s="115">
         <v>0.0</v>
@@ -5067,25 +5073,25 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="104">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B48" t="n" s="109">
         <v>0.48484848484848486</v>
       </c>
       <c r="C48" t="n" s="110">
-        <v>0.0</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="D48" t="n" s="111">
-        <v>0.030303030303030304</v>
+        <v>0.0</v>
       </c>
       <c r="E48" t="n" s="112">
-        <v>0.09090909090909091</v>
+        <v>0.0</v>
       </c>
       <c r="F48" t="n" s="113">
-        <v>0.09090909090909091</v>
+        <v>0.0</v>
       </c>
       <c r="G48" t="n" s="114">
-        <v>0.30303030303030304</v>
+        <v>0.0</v>
       </c>
       <c r="H48" t="n" s="115">
         <v>0.0</v>
@@ -5093,25 +5099,25 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="104">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B49" t="n" s="109">
-        <v>0.16161616161616163</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="C49" t="n" s="110">
-        <v>0.16161616161616163</v>
+        <v>0.0</v>
       </c>
       <c r="D49" t="n" s="111">
-        <v>0.030303030303030304</v>
+        <v>0.0</v>
       </c>
       <c r="E49" t="n" s="112">
-        <v>0.3838383838383838</v>
+        <v>0.08080808080808081</v>
       </c>
       <c r="F49" t="n" s="113">
-        <v>0.2222222222222222</v>
+        <v>0.23232323232323232</v>
       </c>
       <c r="G49" t="n" s="114">
-        <v>0.04040404040404041</v>
+        <v>0.20202020202020202</v>
       </c>
       <c r="H49" t="n" s="115">
         <v>0.0</v>
@@ -5119,25 +5125,25 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="104">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B50" t="n" s="109">
-        <v>0.16161616161616163</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="C50" t="n" s="110">
-        <v>0.21212121212121213</v>
+        <v>0.0</v>
       </c>
       <c r="D50" t="n" s="111">
+        <v>0.030303030303030304</v>
+      </c>
+      <c r="E50" t="n" s="112">
         <v>0.09090909090909091</v>
       </c>
-      <c r="E50" t="n" s="112">
-        <v>0.26262626262626265</v>
-      </c>
       <c r="F50" t="n" s="113">
-        <v>0.050505050505050504</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="G50" t="n" s="114">
-        <v>0.2222222222222222</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="H50" t="n" s="115">
         <v>0.0</v>
@@ -5145,22 +5151,22 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="104">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B51" t="n" s="109">
-        <v>0.32323232323232326</v>
+        <v>0.16161616161616163</v>
       </c>
       <c r="C51" t="n" s="110">
-        <v>0.06060606060606061</v>
+        <v>0.8383838383838383</v>
       </c>
       <c r="D51" t="n" s="111">
-        <v>0.09090909090909091</v>
+        <v>0.0</v>
       </c>
       <c r="E51" t="n" s="112">
-        <v>0.26262626262626265</v>
+        <v>0.0</v>
       </c>
       <c r="F51" t="n" s="113">
-        <v>0.26262626262626265</v>
+        <v>0.0</v>
       </c>
       <c r="G51" t="n" s="114">
         <v>0.0</v>
@@ -5171,25 +5177,25 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="104">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B52" t="n" s="109">
-        <v>0.1414141414141414</v>
+        <v>0.16161616161616163</v>
       </c>
       <c r="C52" t="n" s="110">
+        <v>0.16161616161616163</v>
+      </c>
+      <c r="D52" t="n" s="111">
         <v>0.030303030303030304</v>
       </c>
-      <c r="D52" t="n" s="111">
-        <v>0.0707070707070707</v>
-      </c>
       <c r="E52" t="n" s="112">
-        <v>0.47474747474747475</v>
+        <v>0.3838383838383838</v>
       </c>
       <c r="F52" t="n" s="113">
-        <v>0.2828282828282828</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="G52" t="n" s="114">
-        <v>0.0</v>
+        <v>0.04040404040404041</v>
       </c>
       <c r="H52" t="n" s="115">
         <v>0.0</v>
@@ -5197,25 +5203,25 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="104">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B53" t="n" s="109">
-        <v>0.10101010101010101</v>
+        <v>0.16161616161616163</v>
       </c>
       <c r="C53" t="n" s="110">
-        <v>0.010101010101010102</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="D53" t="n" s="111">
-        <v>0.30303030303030304</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="E53" t="n" s="112">
+        <v>0.26262626262626265</v>
+      </c>
+      <c r="F53" t="n" s="113">
+        <v>0.050505050505050504</v>
+      </c>
+      <c r="G53" t="n" s="114">
         <v>0.2222222222222222</v>
-      </c>
-      <c r="F53" t="n" s="113">
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="G53" t="n" s="114">
-        <v>0.0</v>
       </c>
       <c r="H53" t="n" s="115">
         <v>0.0</v>
@@ -5223,27 +5229,105 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="104">
+        <v>27</v>
+      </c>
+      <c r="B54" t="n" s="109">
+        <v>0.32323232323232326</v>
+      </c>
+      <c r="C54" t="n" s="110">
+        <v>0.06060606060606061</v>
+      </c>
+      <c r="D54" t="n" s="111">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="E54" t="n" s="112">
+        <v>0.26262626262626265</v>
+      </c>
+      <c r="F54" t="n" s="113">
+        <v>0.26262626262626265</v>
+      </c>
+      <c r="G54" t="n" s="114">
+        <v>0.0</v>
+      </c>
+      <c r="H54" t="n" s="115">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="104">
+        <v>28</v>
+      </c>
+      <c r="B55" t="n" s="109">
+        <v>0.1414141414141414</v>
+      </c>
+      <c r="C55" t="n" s="110">
+        <v>0.030303030303030304</v>
+      </c>
+      <c r="D55" t="n" s="111">
+        <v>0.0707070707070707</v>
+      </c>
+      <c r="E55" t="n" s="112">
+        <v>0.47474747474747475</v>
+      </c>
+      <c r="F55" t="n" s="113">
+        <v>0.2828282828282828</v>
+      </c>
+      <c r="G55" t="n" s="114">
+        <v>0.0</v>
+      </c>
+      <c r="H55" t="n" s="115">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="104">
         <v>29</v>
       </c>
-      <c r="B54" t="n" s="109">
+      <c r="B56" t="n" s="109">
+        <v>0.10101010101010101</v>
+      </c>
+      <c r="C56" t="n" s="110">
+        <v>0.010101010101010102</v>
+      </c>
+      <c r="D56" t="n" s="111">
+        <v>0.30303030303030304</v>
+      </c>
+      <c r="E56" t="n" s="112">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="F56" t="n" s="113">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="G56" t="n" s="114">
+        <v>0.0</v>
+      </c>
+      <c r="H56" t="n" s="115">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="104">
+        <v>30</v>
+      </c>
+      <c r="B57" t="n" s="109">
         <v>0.13131313131313133</v>
       </c>
-      <c r="C54" t="n" s="110">
+      <c r="C57" t="n" s="110">
         <v>0.010101010101010102</v>
       </c>
-      <c r="D54" t="n" s="111">
+      <c r="D57" t="n" s="111">
         <v>0.41414141414141414</v>
       </c>
-      <c r="E54" t="n" s="112">
+      <c r="E57" t="n" s="112">
         <v>0.24242424242424243</v>
       </c>
-      <c r="F54" t="n" s="113">
+      <c r="F57" t="n" s="113">
         <v>0.20202020202020202</v>
       </c>
-      <c r="G54" t="n" s="114">
-        <v>0.0</v>
-      </c>
-      <c r="H54" t="n" s="115">
+      <c r="G57" t="n" s="114">
+        <v>0.0</v>
+      </c>
+      <c r="H57" t="n" s="115">
         <v>0.0</v>
       </c>
     </row>
@@ -5274,7 +5358,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="117">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
@@ -5323,31 +5407,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="146">
-        <v>0.8359761208326919</v>
+        <v>0.866997920036977</v>
       </c>
       <c r="B6" t="n" s="147">
-        <v>0.838886673547712</v>
+        <v>0.9881848332269476</v>
       </c>
       <c r="C6" t="n" s="148">
-        <v>0.8294331041027809</v>
+        <v>0.9839136309249329</v>
       </c>
       <c r="D6" t="n" s="149">
-        <v>0.5655390437945523</v>
+        <v>0.965372753075453</v>
       </c>
       <c r="E6" t="n" s="150">
-        <v>5.206811205627606</v>
+        <v>83.63697713355671</v>
       </c>
       <c r="F6" t="n" s="151">
-        <v>0.027475141886540974</v>
+        <v>0.003156805612641833</v>
       </c>
       <c r="G6" t="n" s="152">
-        <v>4.202020202020202</v>
+        <v>1.6363636363636362</v>
       </c>
       <c r="H6" t="n" s="153">
-        <v>0.70861748093142</v>
+        <v>1.6358310134346192</v>
       </c>
       <c r="I6" t="n" s="154">
-        <v>0.554295449339048</v>
+        <v>0.9708245213256605</v>
       </c>
     </row>
     <row r="7">
@@ -5394,118 +5478,88 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="168">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B11" t="n" s="173">
-        <v>0.7930504045853</v>
+        <v>0.984893111638955</v>
       </c>
       <c r="C11" t="n" s="174">
-        <v>0.7936873944308467</v>
+        <v>0.9851963082665955</v>
       </c>
       <c r="D11" t="n" s="175">
-        <v>0.7228046656624423</v>
+        <v>0.9708245213256605</v>
       </c>
       <c r="E11" t="n" s="176">
-        <v>0.5618527746586698</v>
+        <v>0.9708245213256605</v>
       </c>
       <c r="F11" t="n" s="177">
-        <v>3.8470135755462276</v>
+        <v>66.55071761886975</v>
       </c>
       <c r="G11" t="n" s="178">
-        <v>0.0355633080179081</v>
-      </c>
-      <c r="H11" t="n" s="179">
-        <v>0.0024029777513930256</v>
-      </c>
+        <v>0.0030050468619000387</v>
+      </c>
+      <c r="H11" s="179"/>
       <c r="I11" t="n" s="180">
-        <v>0.5646885082722398</v>
+        <v>0.9708245213256605</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="168">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B12" t="n" s="173">
-        <v>0.7962221332265387</v>
+        <v>0.5742379547689282</v>
       </c>
       <c r="C12" t="n" s="174">
-        <v>0.8030737358798807</v>
+        <v>0.9756830184628724</v>
       </c>
       <c r="D12" t="n" s="175">
-        <v>0.7667150361311699</v>
+        <v>0.9525205927941633</v>
       </c>
       <c r="E12" t="n" s="176">
-        <v>0.5761540188858962</v>
+        <v>0.9525205927941631</v>
       </c>
       <c r="F12" t="n" s="177">
-        <v>4.078042811953356</v>
+        <v>40.12352507539585</v>
       </c>
       <c r="G12" t="n" s="178">
-        <v>0.036903759738358376</v>
-      </c>
-      <c r="H12" t="n" s="179">
-        <v>0.025376425381324938</v>
-      </c>
+        <v>0.01203743210370022</v>
+      </c>
+      <c r="H12" s="179"/>
       <c r="I12" t="n" s="180">
-        <v>0.5646885082722398</v>
+        <v>0.9525205927941631</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="168">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B13" t="n" s="173">
-        <v>0.7692209450830142</v>
+        <v>0.5959648215209519</v>
       </c>
       <c r="C13" t="n" s="174">
-        <v>0.7685763700884358</v>
+        <v>0.9861986894129204</v>
       </c>
       <c r="D13" t="n" s="175">
-        <v>0.7014934781232127</v>
+        <v>0.9727731451065351</v>
       </c>
       <c r="E13" t="n" s="176">
-        <v>0.5253975525656478</v>
+        <v>0.9727731451065349</v>
       </c>
       <c r="F13" t="n" s="177">
-        <v>3.3210799190304745</v>
+        <v>71.45688687972672</v>
       </c>
       <c r="G13" t="n" s="178">
-        <v>0.040018508973581564</v>
-      </c>
-      <c r="H13" t="n" s="179">
-        <v>0.008952085247256722</v>
-      </c>
+        <v>0.009070648901941931</v>
+      </c>
+      <c r="H13" s="179"/>
       <c r="I13" t="n" s="180">
-        <v>0.5439023904058561</v>
+        <v>0.972773145106535</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="168">
-        <v>21</v>
-      </c>
-      <c r="B14" t="n" s="173">
-        <v>0.812809826716385</v>
-      </c>
-      <c r="C14" t="n" s="174">
-        <v>0.8174072796436851</v>
-      </c>
-      <c r="D14" t="n" s="175">
-        <v>0.7684196343741401</v>
-      </c>
-      <c r="E14" t="n" s="176">
-        <v>0.5987518290679957</v>
-      </c>
-      <c r="F14" t="n" s="177">
-        <v>4.476669595855633</v>
-      </c>
-      <c r="G14" t="n" s="178">
-        <v>0.03344434244156696</v>
-      </c>
-      <c r="H14" t="n" s="179">
-        <v>0.015412496023596997</v>
-      </c>
-      <c r="I14" t="n" s="180">
-        <v>0.5439023904058561</v>
+      <c r="A14" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -5514,283 +5568,226 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>1</v>
+      <c r="A16" t="s" s="184">
+        <v>31</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="184">
-        <v>30</v>
+      <c r="A17"/>
+      <c r="B17" t="s" s="198">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s" s="198">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s" s="198">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s" s="198">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s" s="198">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s" s="198">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s" s="198">
+        <v>10</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18"/>
-      <c r="B18" t="s" s="198">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s" s="198">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s" s="198">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s" s="198">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s" s="198">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s" s="198">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s" s="198">
-        <v>10</v>
+      <c r="A18" t="s" s="194">
+        <v>21</v>
+      </c>
+      <c r="B18" t="n" s="199">
+        <v>99.0</v>
+      </c>
+      <c r="C18" t="n" s="200">
+        <v>0.9753971277476351</v>
+      </c>
+      <c r="D18" t="n" s="201">
+        <v>0.986551588619224</v>
+      </c>
+      <c r="E18" t="n" s="202">
+        <v>0.9767124118924404</v>
+      </c>
+      <c r="F18" t="n" s="203">
+        <v>0.9695662348731334</v>
+      </c>
+      <c r="G18" t="n" s="204">
+        <v>0.5151515151515151</v>
+      </c>
+      <c r="H18" t="n" s="205">
+        <v>0.5023137559951615</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="194">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" t="n" s="199">
         <v>99.0</v>
       </c>
       <c r="C19" t="n" s="200">
-        <v>0.8133407735252237</v>
+        <v>0.9931899070036554</v>
       </c>
       <c r="D19" t="n" s="201">
-        <v>0.8244361858701337</v>
+        <v>0.9927245652118859</v>
       </c>
       <c r="E19" t="n" s="202">
-        <v>0.7695279608704744</v>
+        <v>0.9897222896110233</v>
       </c>
       <c r="F19" t="n" s="203">
-        <v>0.6663640427694105</v>
+        <v>0.9781032341391557</v>
       </c>
       <c r="G19" t="n" s="204">
-        <v>3.888888888888889</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="H19" t="n" s="205">
-        <v>0.8316309141225229</v>
+        <v>2.1869913932980913</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="194">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" t="n" s="199">
         <v>99.0</v>
       </c>
       <c r="C20" t="n" s="200">
-        <v>0.8213464914660009</v>
+        <v>0.9915777940215159</v>
       </c>
       <c r="D20" t="n" s="201">
-        <v>0.8113728095535923</v>
+        <v>0.9858944177301144</v>
       </c>
       <c r="E20" t="n" s="202">
-        <v>0.7141303350177266</v>
+        <v>0.9747897640587289</v>
       </c>
       <c r="F20" t="n" s="203">
-        <v>0.6600678773322992</v>
+        <v>0.9714314796844777</v>
       </c>
       <c r="G20" t="n" s="204">
-        <v>4.474747474747475</v>
+        <v>2.212121212121212</v>
       </c>
       <c r="H20" t="n" s="205">
-        <v>0.9073783085152335</v>
+        <v>2.264512053909309</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s" s="194">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n" s="199">
-        <v>99.0</v>
-      </c>
-      <c r="C21" t="n" s="200">
-        <v>0.8459044658825929</v>
-      </c>
-      <c r="D21" t="n" s="201">
-        <v>0.8577359657590479</v>
-      </c>
-      <c r="E21" t="n" s="202">
-        <v>0.8167578448349778</v>
-      </c>
-      <c r="F21" t="n" s="203">
-        <v>0.7266740434879317</v>
-      </c>
-      <c r="G21" t="n" s="204">
-        <v>3.9292929292929295</v>
-      </c>
-      <c r="H21" t="n" s="205">
-        <v>0.7986279720912847</v>
+      <c r="A21" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="194">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="209">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24" t="s" s="223">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s" s="223">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s" s="223">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s" s="223">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s" s="223">
+        <v>42</v>
+      </c>
+      <c r="G24" t="s" s="223">
+        <v>43</v>
+      </c>
+      <c r="H24" t="s" s="223">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="219">
         <v>21</v>
       </c>
-      <c r="B22" t="n" s="199">
-        <v>99.0</v>
-      </c>
-      <c r="C22" t="n" s="200">
-        <v>0.8024075438080372</v>
-      </c>
-      <c r="D22" t="n" s="201">
-        <v>0.7907309903070868</v>
-      </c>
-      <c r="E22" t="n" s="202">
-        <v>0.6906796570474534</v>
-      </c>
-      <c r="F22" t="n" s="203">
-        <v>0.6253655735766824</v>
-      </c>
-      <c r="G22" t="n" s="204">
-        <v>4.515151515151516</v>
-      </c>
-      <c r="H22" t="n" s="205">
-        <v>0.9187795405622853</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="209">
-        <v>36</v>
+      <c r="B25" t="n" s="224">
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="C25" t="n" s="225">
+        <v>0.5151515151515151</v>
+      </c>
+      <c r="D25" t="n" s="226">
+        <v>0.0</v>
+      </c>
+      <c r="E25" t="n" s="227">
+        <v>0.0</v>
+      </c>
+      <c r="F25" t="n" s="228">
+        <v>0.0</v>
+      </c>
+      <c r="G25" t="n" s="229">
+        <v>0.0</v>
+      </c>
+      <c r="H25" t="n" s="230">
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26"/>
-      <c r="B26" t="s" s="223">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s" s="223">
-        <v>38</v>
-      </c>
-      <c r="D26" t="s" s="223">
-        <v>39</v>
-      </c>
-      <c r="E26" t="s" s="223">
-        <v>40</v>
-      </c>
-      <c r="F26" t="s" s="223">
-        <v>41</v>
-      </c>
-      <c r="G26" t="s" s="223">
-        <v>42</v>
-      </c>
-      <c r="H26" t="s" s="223">
-        <v>43</v>
+      <c r="A26" t="s" s="219">
+        <v>22</v>
+      </c>
+      <c r="B26" t="n" s="224">
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="C26" t="n" s="225">
+        <v>0.0</v>
+      </c>
+      <c r="D26" t="n" s="226">
+        <v>0.0</v>
+      </c>
+      <c r="E26" t="n" s="227">
+        <v>0.08080808080808081</v>
+      </c>
+      <c r="F26" t="n" s="228">
+        <v>0.23232323232323232</v>
+      </c>
+      <c r="G26" t="n" s="229">
+        <v>0.20202020202020202</v>
+      </c>
+      <c r="H26" t="n" s="230">
+        <v>0.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="219">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B27" t="n" s="224">
-        <v>0.010101010101010102</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="C27" t="n" s="225">
-        <v>0.010101010101010102</v>
+        <v>0.0</v>
       </c>
       <c r="D27" t="n" s="226">
-        <v>0.0</v>
+        <v>0.030303030303030304</v>
       </c>
       <c r="E27" t="n" s="227">
-        <v>0.24242424242424243</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="F27" t="n" s="228">
-        <v>0.5353535353535354</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="G27" t="n" s="229">
-        <v>0.20202020202020202</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="H27" t="n" s="230">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="219">
-        <v>19</v>
-      </c>
-      <c r="B28" t="n" s="224">
-        <v>0.010101010101010102</v>
-      </c>
-      <c r="C28" t="n" s="225">
-        <v>0.0</v>
-      </c>
-      <c r="D28" t="n" s="226">
-        <v>0.0</v>
-      </c>
-      <c r="E28" t="n" s="227">
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="F28" t="n" s="228">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="G28" t="n" s="229">
-        <v>0.696969696969697</v>
-      </c>
-      <c r="H28" t="n" s="230">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="219">
-        <v>20</v>
-      </c>
-      <c r="B29" t="n" s="224">
-        <v>0.0</v>
-      </c>
-      <c r="C29" t="n" s="225">
-        <v>0.020202020202020204</v>
-      </c>
-      <c r="D29" t="n" s="226">
-        <v>0.010101010101010102</v>
-      </c>
-      <c r="E29" t="n" s="227">
-        <v>0.20202020202020202</v>
-      </c>
-      <c r="F29" t="n" s="228">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="G29" t="n" s="229">
-        <v>0.21212121212121213</v>
-      </c>
-      <c r="H29" t="n" s="230">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="219">
-        <v>21</v>
-      </c>
-      <c r="B30" t="n" s="224">
-        <v>0.0</v>
-      </c>
-      <c r="C30" t="n" s="225">
-        <v>0.010101010101010102</v>
-      </c>
-      <c r="D30" t="n" s="226">
-        <v>0.020202020202020204</v>
-      </c>
-      <c r="E30" t="n" s="227">
-        <v>0.1717171717171717</v>
-      </c>
-      <c r="F30" t="n" s="228">
-        <v>0.04040404040404041</v>
-      </c>
-      <c r="G30" t="n" s="229">
-        <v>0.7575757575757576</v>
-      </c>
-      <c r="H30" t="n" s="230">
         <v>0.0</v>
       </c>
     </row>
@@ -5821,7 +5818,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="232">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
@@ -5870,31 +5867,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="261">
-        <v>0.845127339742878</v>
+        <v>0.753038818455104</v>
       </c>
       <c r="B6" t="n" s="262">
-        <v>0.851470839237203</v>
+        <v>0.8733617047389008</v>
       </c>
       <c r="C6" t="n" s="263">
-        <v>0.741357614874748</v>
+        <v>0.8287048061564057</v>
       </c>
       <c r="D6" t="n" s="264">
-        <v>0.7413576148747478</v>
+        <v>0.6968626968249687</v>
       </c>
       <c r="E6" t="n" s="265">
-        <v>5.732684644983708</v>
+        <v>6.896505539167516</v>
       </c>
       <c r="F6" t="n" s="266">
-        <v>0.03025923981850528</v>
+        <v>0.02231067435381315</v>
       </c>
       <c r="G6" t="n" s="267">
-        <v>2.4797979797979797</v>
+        <v>1.9326599326599327</v>
       </c>
       <c r="H6" t="n" s="268">
-        <v>1.523488196640197</v>
+        <v>1.107570115182282</v>
       </c>
       <c r="I6" t="n" s="269">
-        <v>0.7413576148747479</v>
+        <v>0.7248774174052455</v>
       </c>
     </row>
     <row r="7">
@@ -5944,22 +5941,24 @@
         <v>24</v>
       </c>
       <c r="B11" t="n" s="288">
-        <v>0.7413576148747479</v>
+        <v>0.845127339742878</v>
       </c>
       <c r="C11" t="n" s="289">
-        <v>0.7413576148747479</v>
+        <v>0.851470839237203</v>
       </c>
       <c r="D11" t="n" s="290">
-        <v>0.5496111131327752</v>
+        <v>0.741357614874748</v>
       </c>
       <c r="E11" t="n" s="291">
-        <v>0.7413576148747479</v>
-      </c>
-      <c r="F11" s="292"/>
-      <c r="G11" s="293"/>
-      <c r="H11" t="n" s="294">
-        <v>0.7413576148747479</v>
-      </c>
+        <v>0.7413576148747478</v>
+      </c>
+      <c r="F11" t="n" s="292">
+        <v>5.732684644983708</v>
+      </c>
+      <c r="G11" t="n" s="293">
+        <v>0.03025923981850528</v>
+      </c>
+      <c r="H11" s="294"/>
       <c r="I11" t="n" s="295">
         <v>0.7413576148747479</v>
       </c>
@@ -5969,25 +5968,53 @@
         <v>25</v>
       </c>
       <c r="B12" t="n" s="288">
-        <v>0.5496111131327752</v>
+        <v>0.40119790873559724</v>
       </c>
       <c r="C12" t="n" s="289">
-        <v>0.7413576148747479</v>
-      </c>
-      <c r="D12" s="290"/>
-      <c r="E12" s="291"/>
-      <c r="F12" s="292"/>
-      <c r="G12" s="293"/>
-      <c r="H12" t="n" s="294">
-        <v>0.5496111131327752</v>
-      </c>
+        <v>0.7687405826523139</v>
+      </c>
+      <c r="D12" t="n" s="290">
+        <v>0.6243530581949126</v>
+      </c>
+      <c r="E12" t="n" s="291">
+        <v>0.6243530581949126</v>
+      </c>
+      <c r="F12" t="n" s="292">
+        <v>3.3241482291575357</v>
+      </c>
+      <c r="G12" t="n" s="293">
+        <v>0.03903755581171379</v>
+      </c>
+      <c r="H12" s="294"/>
       <c r="I12" t="n" s="295">
-        <v>0.7413576148747479</v>
+        <v>0.6243530581949127</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>1</v>
+      <c r="A13" t="s" s="283">
+        <v>26</v>
+      </c>
+      <c r="B13" t="n" s="288">
+        <v>0.5040996836464586</v>
+      </c>
+      <c r="C13" t="n" s="289">
+        <v>0.8404973131316051</v>
+      </c>
+      <c r="D13" t="n" s="290">
+        <v>0.7248774174052455</v>
+      </c>
+      <c r="E13" t="n" s="291">
+        <v>0.7248774174052455</v>
+      </c>
+      <c r="F13" t="n" s="292">
+        <v>5.269486863409997</v>
+      </c>
+      <c r="G13" t="n" s="293">
+        <v>0.03390577597001988</v>
+      </c>
+      <c r="H13" s="294"/>
+      <c r="I13" t="n" s="295">
+        <v>0.7248774174052455</v>
       </c>
     </row>
     <row r="14">
@@ -5996,174 +6023,231 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="299">
-        <v>30</v>
+      <c r="A15" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16"/>
-      <c r="B16" t="s" s="313">
+      <c r="A16" t="s" s="299">
         <v>31</v>
       </c>
-      <c r="C16" t="s" s="313">
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s" s="313">
         <v>32</v>
       </c>
-      <c r="D16" t="s" s="313">
+      <c r="C17" t="s" s="313">
         <v>33</v>
       </c>
-      <c r="E16" t="s" s="313">
+      <c r="D17" t="s" s="313">
         <v>34</v>
       </c>
-      <c r="F16" t="s" s="313">
+      <c r="E17" t="s" s="313">
         <v>35</v>
       </c>
-      <c r="G16" t="s" s="313">
+      <c r="F17" t="s" s="313">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s" s="313">
         <v>9</v>
       </c>
-      <c r="H16" t="s" s="313">
+      <c r="H17" t="s" s="313">
         <v>10</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="309">
-        <v>24</v>
-      </c>
-      <c r="B17" t="n" s="314">
-        <v>99.0</v>
-      </c>
-      <c r="C17" t="n" s="315">
-        <v>0.9214899206740435</v>
-      </c>
-      <c r="D17" t="n" s="316">
-        <v>0.9331017133396412</v>
-      </c>
-      <c r="E17" t="n" s="317">
-        <v>0.8034204154760828</v>
-      </c>
-      <c r="F17" t="n" s="318">
-        <v>0.7413576148747479</v>
-      </c>
-      <c r="G17" t="n" s="319">
-        <v>2.4646464646464645</v>
-      </c>
-      <c r="H17" t="n" s="320">
-        <v>1.5004294032527945</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="309">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="n" s="314">
         <v>99.0</v>
       </c>
       <c r="C18" t="n" s="315">
-        <v>0.943814293244623</v>
+        <v>0.7700336761104424</v>
       </c>
       <c r="D18" t="n" s="316">
-        <v>0.9331017133396412</v>
+        <v>0.8766532259301054</v>
       </c>
       <c r="E18" t="n" s="317">
-        <v>0.8034204154760828</v>
+        <v>0.7753560799764248</v>
       </c>
       <c r="F18" t="n" s="318">
-        <v>0.7413576148747476</v>
+        <v>0.7182947837745781</v>
       </c>
       <c r="G18" t="n" s="319">
+        <v>0.8383838383838383</v>
+      </c>
+      <c r="H18" t="n" s="320">
+        <v>0.3699716124540519</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="309">
+        <v>25</v>
+      </c>
+      <c r="B19" t="n" s="314">
+        <v>99.0</v>
+      </c>
+      <c r="C19" t="n" s="315">
+        <v>0.9257328451789401</v>
+      </c>
+      <c r="D19" t="n" s="316">
+        <v>0.9203153625860224</v>
+      </c>
+      <c r="E19" t="n" s="317">
+        <v>0.8724599391707504</v>
+      </c>
+      <c r="F19" t="n" s="318">
+        <v>0.7817959382204099</v>
+      </c>
+      <c r="G19" t="n" s="319">
+        <v>2.4646464646464645</v>
+      </c>
+      <c r="H19" t="n" s="320">
+        <v>1.5004294032527945</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="309">
+        <v>26</v>
+      </c>
+      <c r="B20" t="n" s="314">
+        <v>99.0</v>
+      </c>
+      <c r="C20" t="n" s="315">
+        <v>0.9350116187532647</v>
+      </c>
+      <c r="D20" t="n" s="316">
+        <v>0.8828030773072519</v>
+      </c>
+      <c r="E20" t="n" s="317">
+        <v>0.7916665520160241</v>
+      </c>
+      <c r="F20" t="n" s="318">
+        <v>0.7517827808997651</v>
+      </c>
+      <c r="G20" t="n" s="319">
         <v>2.494949494949495</v>
       </c>
-      <c r="H18" t="n" s="320">
+      <c r="H20" t="n" s="320">
         <v>1.7634251074735523</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="21">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="22">
+      <c r="A22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="324">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22"/>
-      <c r="B22" t="s" s="338">
+    <row r="23">
+      <c r="A23" t="s" s="324">
         <v>37</v>
       </c>
-      <c r="C22" t="s" s="338">
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24" t="s" s="338">
         <v>38</v>
       </c>
-      <c r="D22" t="s" s="338">
+      <c r="C24" t="s" s="338">
         <v>39</v>
       </c>
-      <c r="E22" t="s" s="338">
+      <c r="D24" t="s" s="338">
         <v>40</v>
       </c>
-      <c r="F22" t="s" s="338">
+      <c r="E24" t="s" s="338">
         <v>41</v>
       </c>
-      <c r="G22" t="s" s="338">
+      <c r="F24" t="s" s="338">
         <v>42</v>
       </c>
-      <c r="H22" t="s" s="338">
+      <c r="G24" t="s" s="338">
         <v>43</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="334">
+      <c r="H24" t="s" s="338">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="334">
         <v>24</v>
       </c>
-      <c r="B23" t="n" s="339">
+      <c r="B25" t="n" s="339">
         <v>0.16161616161616163</v>
       </c>
-      <c r="C23" t="n" s="340">
+      <c r="C25" t="n" s="340">
+        <v>0.8383838383838383</v>
+      </c>
+      <c r="D25" t="n" s="341">
+        <v>0.0</v>
+      </c>
+      <c r="E25" t="n" s="342">
+        <v>0.0</v>
+      </c>
+      <c r="F25" t="n" s="343">
+        <v>0.0</v>
+      </c>
+      <c r="G25" t="n" s="344">
+        <v>0.0</v>
+      </c>
+      <c r="H25" t="n" s="345">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="334">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n" s="339">
         <v>0.16161616161616163</v>
       </c>
-      <c r="D23" t="n" s="341">
+      <c r="C26" t="n" s="340">
+        <v>0.16161616161616163</v>
+      </c>
+      <c r="D26" t="n" s="341">
         <v>0.030303030303030304</v>
       </c>
-      <c r="E23" t="n" s="342">
+      <c r="E26" t="n" s="342">
         <v>0.3838383838383838</v>
       </c>
-      <c r="F23" t="n" s="343">
+      <c r="F26" t="n" s="343">
         <v>0.2222222222222222</v>
       </c>
-      <c r="G23" t="n" s="344">
+      <c r="G26" t="n" s="344">
         <v>0.04040404040404041</v>
       </c>
-      <c r="H23" t="n" s="345">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="334">
-        <v>25</v>
-      </c>
-      <c r="B24" t="n" s="339">
+      <c r="H26" t="n" s="345">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="334">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n" s="339">
         <v>0.16161616161616163</v>
       </c>
-      <c r="C24" t="n" s="340">
+      <c r="C27" t="n" s="340">
         <v>0.21212121212121213</v>
       </c>
-      <c r="D24" t="n" s="341">
+      <c r="D27" t="n" s="341">
         <v>0.09090909090909091</v>
       </c>
-      <c r="E24" t="n" s="342">
+      <c r="E27" t="n" s="342">
         <v>0.26262626262626265</v>
       </c>
-      <c r="F24" t="n" s="343">
+      <c r="F27" t="n" s="343">
         <v>0.050505050505050504</v>
       </c>
-      <c r="G24" t="n" s="344">
+      <c r="G27" t="n" s="344">
         <v>0.2222222222222222</v>
       </c>
-      <c r="H24" t="n" s="345">
+      <c r="H27" t="n" s="345">
         <v>0.0</v>
       </c>
     </row>
@@ -6194,7 +6278,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="347">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
@@ -6243,31 +6327,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="376">
-        <v>0.8854613835808989</v>
+        <v>0.5910058977719528</v>
       </c>
       <c r="B6" t="n" s="377">
-        <v>0.885742493179992</v>
+        <v>0.7548111898539915</v>
       </c>
       <c r="C6" t="n" s="378">
-        <v>0.7949172321107554</v>
+        <v>0.6739628545052403</v>
       </c>
       <c r="D6" t="n" s="379">
-        <v>0.7949172321107554</v>
+        <v>0.5064563366874081</v>
       </c>
       <c r="E6" t="n" s="380">
-        <v>7.752160167255516</v>
+        <v>3.078489550173625</v>
       </c>
       <c r="F6" t="n" s="381">
-        <v>0.02298756031057443</v>
+        <v>0.04248065514323658</v>
       </c>
       <c r="G6" t="n" s="382">
-        <v>2.5555555555555554</v>
+        <v>3.117845117845118</v>
       </c>
       <c r="H6" t="n" s="383">
-        <v>1.1647214103461911</v>
+        <v>0.5287925991870028</v>
       </c>
       <c r="I6" t="n" s="384">
-        <v>0.7949172321107554</v>
+        <v>0.5006931620309719</v>
       </c>
     </row>
     <row r="7">
@@ -6314,53 +6398,83 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="398">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B11" t="n" s="403">
-        <v>0.7949172321107554</v>
+        <v>0.7028505868855355</v>
       </c>
       <c r="C11" t="n" s="404">
-        <v>0.7949172321107554</v>
+        <v>0.7045813178161824</v>
       </c>
       <c r="D11" t="n" s="405">
-        <v>0.6318934059066246</v>
+        <v>0.5439023904058562</v>
       </c>
       <c r="E11" t="n" s="406">
-        <v>0.7949172321107554</v>
-      </c>
-      <c r="F11" s="407"/>
-      <c r="G11" s="408"/>
-      <c r="H11" t="n" s="409">
-        <v>0.7949172321107554</v>
-      </c>
+        <v>0.5439023904058562</v>
+      </c>
+      <c r="F11" t="n" s="407">
+        <v>2.385026270538208</v>
+      </c>
+      <c r="G11" t="n" s="408">
+        <v>0.05940878948733907</v>
+      </c>
+      <c r="H11" s="409"/>
       <c r="I11" t="n" s="410">
-        <v>0.7949172321107554</v>
+        <v>0.5439023904058561</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="398">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B12" t="n" s="403">
-        <v>0.6318934059066246</v>
+        <v>0.19750334373606782</v>
       </c>
       <c r="C12" t="n" s="404">
-        <v>0.7949172321107554</v>
-      </c>
-      <c r="D12" s="405"/>
-      <c r="E12" s="406"/>
-      <c r="F12" s="407"/>
-      <c r="G12" s="408"/>
-      <c r="H12" t="n" s="409">
-        <v>0.6318934059066246</v>
-      </c>
+        <v>0.6672825261006132</v>
+      </c>
+      <c r="D12" t="n" s="405">
+        <v>0.500693162030972</v>
+      </c>
+      <c r="E12" t="n" s="406">
+        <v>0.5006931620309718</v>
+      </c>
+      <c r="F12" t="n" s="407">
+        <v>2.0055529944976622</v>
+      </c>
+      <c r="G12" t="n" s="408">
+        <v>0.03074231155154791</v>
+      </c>
+      <c r="H12" s="409"/>
       <c r="I12" t="n" s="410">
-        <v>0.7949172321107554</v>
+        <v>0.5006931620309719</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>1</v>
+      <c r="A13" t="s" s="398">
+        <v>20</v>
+      </c>
+      <c r="B13" t="n" s="403">
+        <v>0.20321984692531014</v>
+      </c>
+      <c r="C13" t="n" s="404">
+        <v>0.6438595096359434</v>
+      </c>
+      <c r="D13" t="n" s="405">
+        <v>0.474773457625396</v>
+      </c>
+      <c r="E13" t="n" s="406">
+        <v>0.47477345762539613</v>
+      </c>
+      <c r="F13" t="n" s="407">
+        <v>1.8078806736571078</v>
+      </c>
+      <c r="G13" t="n" s="408">
+        <v>0.03379615815588576</v>
+      </c>
+      <c r="H13" s="409"/>
+      <c r="I13" t="n" s="410">
+        <v>0.4747734576253961</v>
       </c>
     </row>
     <row r="14">
@@ -6369,165 +6483,219 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="414">
-        <v>30</v>
+      <c r="A15" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16"/>
-      <c r="B16" t="s" s="428">
+      <c r="A16" t="s" s="414">
         <v>31</v>
       </c>
-      <c r="C16" t="s" s="428">
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s" s="428">
         <v>32</v>
       </c>
-      <c r="D16" t="s" s="428">
+      <c r="C17" t="s" s="428">
         <v>33</v>
       </c>
-      <c r="E16" t="s" s="428">
+      <c r="D17" t="s" s="428">
         <v>34</v>
       </c>
-      <c r="F16" t="s" s="428">
+      <c r="E17" t="s" s="428">
         <v>35</v>
       </c>
-      <c r="G16" t="s" s="428">
+      <c r="F17" t="s" s="428">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s" s="428">
         <v>9</v>
       </c>
-      <c r="H16" t="s" s="428">
+      <c r="H17" t="s" s="428">
         <v>10</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="424">
-        <v>28</v>
-      </c>
-      <c r="B17" t="n" s="429">
-        <v>99.0</v>
-      </c>
-      <c r="C17" t="n" s="430">
-        <v>0.949154276531876</v>
-      </c>
-      <c r="D17" t="n" s="431">
-        <v>0.9473429242124404</v>
-      </c>
-      <c r="E17" t="n" s="432">
-        <v>0.8446332452660681</v>
-      </c>
-      <c r="F17" t="n" s="433">
-        <v>0.7949172321107554</v>
-      </c>
-      <c r="G17" t="n" s="434">
-        <v>2.7373737373737375</v>
-      </c>
-      <c r="H17" t="n" s="435">
-        <v>1.2501906677918566</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="424">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B18" t="n" s="429">
         <v>99.0</v>
       </c>
       <c r="C18" t="n" s="430">
-        <v>0.9455007415668493</v>
+        <v>0.5986330507152257</v>
       </c>
       <c r="D18" t="n" s="431">
-        <v>0.9473429242124404</v>
+        <v>0.8038899534730961</v>
       </c>
       <c r="E18" t="n" s="432">
-        <v>0.8446332452660681</v>
+        <v>0.6366436988393307</v>
       </c>
       <c r="F18" t="n" s="433">
-        <v>0.7949172321107554</v>
+        <v>0.5556076046501767</v>
       </c>
       <c r="G18" t="n" s="434">
-        <v>2.3737373737373737</v>
+        <v>0.98989898989899</v>
       </c>
       <c r="H18" t="n" s="435">
-        <v>1.208691809150421</v>
+        <v>0.10050378152592121</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="424">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n" s="429">
+        <v>99.0</v>
+      </c>
+      <c r="C19" t="n" s="430">
+        <v>0.8654134438193761</v>
+      </c>
+      <c r="D19" t="n" s="431">
+        <v>0.8214733761653694</v>
+      </c>
+      <c r="E19" t="n" s="432">
+        <v>0.6786976561809229</v>
+      </c>
+      <c r="F19" t="n" s="433">
+        <v>0.5628300793259162</v>
+      </c>
+      <c r="G19" t="n" s="434">
+        <v>3.888888888888889</v>
+      </c>
+      <c r="H19" t="n" s="435">
+        <v>0.8316309141225229</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="424">
+        <v>20</v>
+      </c>
+      <c r="B20" t="n" s="429">
+        <v>99.0</v>
+      </c>
+      <c r="C20" t="n" s="430">
+        <v>0.8888336113743031</v>
+      </c>
+      <c r="D20" t="n" s="431">
+        <v>0.8320210562736059</v>
+      </c>
+      <c r="E20" t="n" s="432">
+        <v>0.7020542714378777</v>
+      </c>
+      <c r="F20" t="n" s="433">
+        <v>0.5687441550442286</v>
+      </c>
+      <c r="G20" t="n" s="434">
+        <v>4.474747474747475</v>
+      </c>
+      <c r="H20" t="n" s="435">
+        <v>0.9073783085152335</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="22">
+      <c r="A22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="439">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22"/>
-      <c r="B22" t="s" s="453">
+    <row r="23">
+      <c r="A23" t="s" s="439">
         <v>37</v>
       </c>
-      <c r="C22" t="s" s="453">
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24" t="s" s="453">
         <v>38</v>
       </c>
-      <c r="D22" t="s" s="453">
+      <c r="C24" t="s" s="453">
         <v>39</v>
       </c>
-      <c r="E22" t="s" s="453">
-        <v>40</v>
-      </c>
-      <c r="F22" t="s" s="453">
+      <c r="D24" t="s" s="453">
         <v>41</v>
       </c>
-      <c r="G22" t="s" s="453">
+      <c r="E24" t="s" s="453">
+        <v>42</v>
+      </c>
+      <c r="F24" t="s" s="453">
         <v>43</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="449">
-        <v>28</v>
-      </c>
-      <c r="B23" t="n" s="454">
-        <v>0.10101010101010101</v>
-      </c>
-      <c r="C23" t="n" s="455">
+      <c r="G24" t="s" s="453">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="449">
+        <v>18</v>
+      </c>
+      <c r="B25" t="n" s="454">
         <v>0.010101010101010102</v>
       </c>
-      <c r="D23" t="n" s="456">
-        <v>0.30303030303030304</v>
-      </c>
-      <c r="E23" t="n" s="457">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="F23" t="n" s="458">
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="G23" t="n" s="459">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="449">
-        <v>29</v>
-      </c>
-      <c r="B24" t="n" s="454">
-        <v>0.13131313131313133</v>
-      </c>
-      <c r="C24" t="n" s="455">
+      <c r="C25" t="n" s="455">
+        <v>0.98989898989899</v>
+      </c>
+      <c r="D25" t="n" s="456">
+        <v>0.0</v>
+      </c>
+      <c r="E25" t="n" s="457">
+        <v>0.0</v>
+      </c>
+      <c r="F25" t="n" s="458">
+        <v>0.0</v>
+      </c>
+      <c r="G25" t="n" s="459">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="449">
+        <v>19</v>
+      </c>
+      <c r="B26" t="n" s="454">
         <v>0.010101010101010102</v>
       </c>
-      <c r="D24" t="n" s="456">
-        <v>0.41414141414141414</v>
-      </c>
-      <c r="E24" t="n" s="457">
+      <c r="C26" t="n" s="455">
+        <v>0.010101010101010102</v>
+      </c>
+      <c r="D26" t="n" s="456">
         <v>0.24242424242424243</v>
       </c>
-      <c r="F24" t="n" s="458">
+      <c r="E26" t="n" s="457">
+        <v>0.5353535353535354</v>
+      </c>
+      <c r="F26" t="n" s="458">
         <v>0.20202020202020202</v>
       </c>
-      <c r="G24" t="n" s="459">
+      <c r="G26" t="n" s="459">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="449">
+        <v>20</v>
+      </c>
+      <c r="B27" t="n" s="454">
+        <v>0.010101010101010102</v>
+      </c>
+      <c r="C27" t="n" s="455">
+        <v>0.0</v>
+      </c>
+      <c r="D27" t="n" s="456">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E27" t="n" s="457">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="F27" t="n" s="458">
+        <v>0.696969696969697</v>
+      </c>
+      <c r="G27" t="n" s="459">
         <v>0.0</v>
       </c>
     </row>
@@ -6558,7 +6726,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="461">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
@@ -6607,31 +6775,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="490">
-        <v>0.984893111638955</v>
+        <v>0.7407714887182375</v>
       </c>
       <c r="B6" t="n" s="491">
-        <v>0.9851963082665955</v>
+        <v>0.75323875272074</v>
       </c>
       <c r="C6" t="n" s="492">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
       <c r="D6" t="n" s="493">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531383</v>
       </c>
       <c r="E6" t="n" s="494">
-        <v>66.55071761886975</v>
+        <v>3.0525001839867465</v>
       </c>
       <c r="F6" t="n" s="495">
-        <v>0.0030050468619000387</v>
+        <v>0.04999699041956449</v>
       </c>
       <c r="G6" t="n" s="496">
-        <v>2.196969696969697</v>
+        <v>2.404040404040404</v>
       </c>
       <c r="H6" t="n" s="497">
-        <v>2.2094626988115693</v>
+        <v>1.3183879451288454</v>
       </c>
       <c r="I6" t="n" s="498">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531383</v>
       </c>
     </row>
     <row r="7">
@@ -6678,48 +6846,48 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="512">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B11" t="n" s="517">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
       <c r="C11" t="n" s="518">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
       <c r="D11" t="n" s="519">
-        <v>0.942500251207198</v>
+        <v>0.36500492261739736</v>
       </c>
       <c r="E11" t="n" s="520">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
       <c r="F11" s="521"/>
       <c r="G11" s="522"/>
       <c r="H11" t="n" s="523">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
       <c r="I11" t="n" s="524">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="512">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n" s="517">
-        <v>0.942500251207198</v>
+        <v>0.36500492261739736</v>
       </c>
       <c r="C12" t="n" s="518">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
       <c r="D12" s="519"/>
       <c r="E12" s="520"/>
       <c r="F12" s="521"/>
       <c r="G12" s="522"/>
       <c r="H12" t="n" s="523">
-        <v>0.942500251207198</v>
+        <v>0.36500492261739736</v>
       </c>
       <c r="I12" t="n" s="524">
-        <v>0.9708245213256605</v>
+        <v>0.6041563726531382</v>
       </c>
     </row>
     <row r="13">
@@ -6734,25 +6902,25 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="528">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s" s="542">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s" s="542">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s" s="542">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s" s="542">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s" s="542">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s" s="542">
         <v>9</v>
@@ -6763,54 +6931,54 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="538">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B17" t="n" s="543">
         <v>99.0</v>
       </c>
       <c r="C17" t="n" s="544">
-        <v>0.9924211950782496</v>
+        <v>0.919583237763186</v>
       </c>
       <c r="D17" t="n" s="545">
-        <v>0.9926793342579617</v>
+        <v>0.8955881789788034</v>
       </c>
       <c r="E17" t="n" s="546">
-        <v>0.9780911952708854</v>
+        <v>0.6961182712982528</v>
       </c>
       <c r="F17" t="n" s="547">
-        <v>0.9708245213256603</v>
+        <v>0.6041563726531383</v>
       </c>
       <c r="G17" t="n" s="548">
-        <v>2.1818181818181817</v>
+        <v>2.080808080808081</v>
       </c>
       <c r="H17" t="n" s="549">
-        <v>2.1869913932980913</v>
+        <v>1.6392928271041933</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="538">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B18" t="n" s="543">
         <v>99.0</v>
       </c>
       <c r="C18" t="n" s="544">
-        <v>0.9929330168849042</v>
+        <v>0.8686568458505952</v>
       </c>
       <c r="D18" t="n" s="545">
-        <v>0.9926793342579617</v>
+        <v>0.8955881789788034</v>
       </c>
       <c r="E18" t="n" s="546">
-        <v>0.9780911952708854</v>
+        <v>0.6961182712982528</v>
       </c>
       <c r="F18" t="n" s="547">
-        <v>0.9708245213256603</v>
+        <v>0.6041563726531383</v>
       </c>
       <c r="G18" t="n" s="548">
-        <v>2.212121212121212</v>
+        <v>2.727272727272727</v>
       </c>
       <c r="H18" t="n" s="549">
-        <v>2.264512053909309</v>
+        <v>1.3000642199065635</v>
       </c>
     </row>
     <row r="19">
@@ -6825,13 +6993,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="553">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="s" s="567">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s" s="567">
         <v>39</v>
@@ -6846,27 +7014,27 @@
         <v>42</v>
       </c>
       <c r="G22" t="s" s="567">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="563">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B23" t="n" s="568">
-        <v>0.48484848484848486</v>
+        <v>0.32323232323232326</v>
       </c>
       <c r="C23" t="n" s="569">
-        <v>0.0</v>
+        <v>0.06060606060606061</v>
       </c>
       <c r="D23" t="n" s="570">
-        <v>0.08080808080808081</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="E23" t="n" s="571">
-        <v>0.23232323232323232</v>
+        <v>0.26262626262626265</v>
       </c>
       <c r="F23" t="n" s="572">
-        <v>0.20202020202020202</v>
+        <v>0.26262626262626265</v>
       </c>
       <c r="G23" t="n" s="573">
         <v>0.0</v>
@@ -6874,22 +7042,22 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="563">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B24" t="n" s="568">
-        <v>0.48484848484848486</v>
+        <v>0.1414141414141414</v>
       </c>
       <c r="C24" t="n" s="569">
         <v>0.030303030303030304</v>
       </c>
       <c r="D24" t="n" s="570">
-        <v>0.09090909090909091</v>
+        <v>0.0707070707070707</v>
       </c>
       <c r="E24" t="n" s="571">
-        <v>0.09090909090909091</v>
+        <v>0.47474747474747475</v>
       </c>
       <c r="F24" t="n" s="572">
-        <v>0.30303030303030304</v>
+        <v>0.2828282828282828</v>
       </c>
       <c r="G24" t="n" s="573">
         <v>0.0</v>
@@ -6922,7 +7090,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="575">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
@@ -6971,31 +7139,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="604">
-        <v>0.7407714887182375</v>
+        <v>0.8854613835808989</v>
       </c>
       <c r="B6" t="n" s="605">
-        <v>0.75323875272074</v>
+        <v>0.885742493179992</v>
       </c>
       <c r="C6" t="n" s="606">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="D6" t="n" s="607">
-        <v>0.6041563726531383</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="E6" t="n" s="608">
-        <v>3.0525001839867465</v>
+        <v>7.752160167255516</v>
       </c>
       <c r="F6" t="n" s="609">
-        <v>0.04999699041956449</v>
+        <v>0.02298756031057443</v>
       </c>
       <c r="G6" t="n" s="610">
-        <v>2.404040404040404</v>
+        <v>2.5555555555555554</v>
       </c>
       <c r="H6" t="n" s="611">
-        <v>1.3183879451288454</v>
+        <v>1.1647214103461911</v>
       </c>
       <c r="I6" t="n" s="612">
-        <v>0.6041563726531383</v>
+        <v>0.7949172321107554</v>
       </c>
     </row>
     <row r="7">
@@ -7042,48 +7210,48 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="626">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" t="n" s="631">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="C11" t="n" s="632">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="D11" t="n" s="633">
-        <v>0.36500492261739736</v>
+        <v>0.6318934059066246</v>
       </c>
       <c r="E11" t="n" s="634">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="F11" s="635"/>
       <c r="G11" s="636"/>
       <c r="H11" t="n" s="637">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="I11" t="n" s="638">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="626">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" t="n" s="631">
-        <v>0.36500492261739736</v>
+        <v>0.6318934059066246</v>
       </c>
       <c r="C12" t="n" s="632">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="D12" s="633"/>
       <c r="E12" s="634"/>
       <c r="F12" s="635"/>
       <c r="G12" s="636"/>
       <c r="H12" t="n" s="637">
-        <v>0.36500492261739736</v>
+        <v>0.6318934059066246</v>
       </c>
       <c r="I12" t="n" s="638">
-        <v>0.6041563726531382</v>
+        <v>0.7949172321107554</v>
       </c>
     </row>
     <row r="13">
@@ -7098,25 +7266,25 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="642">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s" s="656">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s" s="656">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s" s="656">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s" s="656">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s" s="656">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s" s="656">
         <v>9</v>
@@ -7127,54 +7295,54 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="652">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B17" t="n" s="657">
         <v>99.0</v>
       </c>
       <c r="C17" t="n" s="658">
-        <v>0.919583237763186</v>
+        <v>0.949154276531876</v>
       </c>
       <c r="D17" t="n" s="659">
-        <v>0.8955881789788034</v>
+        <v>0.9473429242124404</v>
       </c>
       <c r="E17" t="n" s="660">
-        <v>0.6961182712982528</v>
+        <v>0.8446332452660681</v>
       </c>
       <c r="F17" t="n" s="661">
-        <v>0.6041563726531383</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="G17" t="n" s="662">
-        <v>2.080808080808081</v>
+        <v>2.7373737373737375</v>
       </c>
       <c r="H17" t="n" s="663">
-        <v>1.6392928271041933</v>
+        <v>1.2501906677918566</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="652">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B18" t="n" s="657">
         <v>99.0</v>
       </c>
       <c r="C18" t="n" s="658">
-        <v>0.8686568458505952</v>
+        <v>0.9455007415668493</v>
       </c>
       <c r="D18" t="n" s="659">
-        <v>0.8955881789788034</v>
+        <v>0.9473429242124404</v>
       </c>
       <c r="E18" t="n" s="660">
-        <v>0.6961182712982528</v>
+        <v>0.8446332452660681</v>
       </c>
       <c r="F18" t="n" s="661">
-        <v>0.6041563726531383</v>
+        <v>0.7949172321107554</v>
       </c>
       <c r="G18" t="n" s="662">
-        <v>2.727272727272727</v>
+        <v>2.3737373737373737</v>
       </c>
       <c r="H18" t="n" s="663">
-        <v>1.3000642199065635</v>
+        <v>1.208691809150421</v>
       </c>
     </row>
     <row r="19">
@@ -7189,48 +7357,48 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="667">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="s" s="681">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s" s="681">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s" s="681">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s" s="681">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F22" t="s" s="681">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s" s="681">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="677">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B23" t="n" s="682">
-        <v>0.32323232323232326</v>
+        <v>0.10101010101010101</v>
       </c>
       <c r="C23" t="n" s="683">
-        <v>0.06060606060606061</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="D23" t="n" s="684">
-        <v>0.09090909090909091</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="E23" t="n" s="685">
-        <v>0.26262626262626265</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="F23" t="n" s="686">
-        <v>0.26262626262626265</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="G23" t="n" s="687">
         <v>0.0</v>
@@ -7238,22 +7406,22 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="677">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B24" t="n" s="682">
-        <v>0.1414141414141414</v>
+        <v>0.13131313131313133</v>
       </c>
       <c r="C24" t="n" s="683">
-        <v>0.030303030303030304</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="D24" t="n" s="684">
-        <v>0.0707070707070707</v>
+        <v>0.41414141414141414</v>
       </c>
       <c r="E24" t="n" s="685">
-        <v>0.47474747474747475</v>
+        <v>0.24242424242424243</v>
       </c>
       <c r="F24" t="n" s="686">
-        <v>0.2828282828282828</v>
+        <v>0.20202020202020202</v>
       </c>
       <c r="G24" t="n" s="687">
         <v>0.0</v>
@@ -7286,7 +7454,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="689">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
@@ -7335,31 +7503,31 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="718">
-        <v>0.7954851259812854</v>
+        <v>0.7935038049495212</v>
       </c>
       <c r="B6" t="n" s="719">
-        <v>0.8206757961812295</v>
+        <v>0.8207321794624566</v>
       </c>
       <c r="C6" t="n" s="720">
-        <v>0.9080620499809474</v>
+        <v>0.9055967839156669</v>
       </c>
       <c r="D6" t="n" s="721">
-        <v>0.3139638841705832</v>
+        <v>0.3140464215739184</v>
       </c>
       <c r="E6" t="n" s="722">
-        <v>4.5764920669081866</v>
+        <v>4.578245984145121</v>
       </c>
       <c r="F6" t="n" s="723">
-        <v>0.028651900632429818</v>
+        <v>0.026408811767212974</v>
       </c>
       <c r="G6" t="n" s="724">
-        <v>3.1121212121212123</v>
+        <v>2.418181818181818</v>
       </c>
       <c r="H6" t="n" s="725">
-        <v>0.845549299456135</v>
+        <v>0.8172082436830891</v>
       </c>
       <c r="I6" t="n" s="726">
-        <v>0.2761101265726882</v>
+        <v>0.2751279098582749</v>
       </c>
     </row>
     <row r="7">
@@ -7406,292 +7574,292 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="740">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B11" t="n" s="745">
-        <v>0.7771453241664338</v>
+        <v>0.7753673094582185</v>
       </c>
       <c r="C11" t="n" s="746">
-        <v>0.7924839820480762</v>
+        <v>0.7928988626938881</v>
       </c>
       <c r="D11" t="n" s="747">
-        <v>0.8857568671367618</v>
+        <v>0.8796958510390007</v>
       </c>
       <c r="E11" t="n" s="748">
-        <v>0.2979119573431558</v>
+        <v>0.2984402843082706</v>
       </c>
       <c r="F11" t="n" s="749">
-        <v>3.818905113299133</v>
+        <v>3.8285587081152577</v>
       </c>
       <c r="G11" t="n" s="750">
-        <v>0.031156478631273098</v>
+        <v>0.029870416455644287</v>
       </c>
       <c r="H11" t="n" s="751">
-        <v>0.04075244874554898</v>
+        <v>0.04190318853695907</v>
       </c>
       <c r="I11" t="n" s="752">
-        <v>0.2600359248915194</v>
+        <v>0.2756190182154815</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="740">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B12" t="n" s="745">
-        <v>0.7828362699168575</v>
+        <v>0.7404758211072203</v>
       </c>
       <c r="C12" t="n" s="746">
-        <v>0.8003301792610131</v>
+        <v>0.7866843487089727</v>
       </c>
       <c r="D12" t="n" s="747">
-        <v>0.8975402730329505</v>
+        <v>0.8758064602202362</v>
       </c>
       <c r="E12" t="n" s="748">
-        <v>0.3081323425131442</v>
+        <v>0.2906621175028968</v>
       </c>
       <c r="F12" t="n" s="749">
-        <v>4.0082681313528274</v>
+        <v>3.6878885536424932</v>
       </c>
       <c r="G12" t="n" s="750">
-        <v>0.03006151121404241</v>
+        <v>0.034973671139709644</v>
       </c>
       <c r="H12" t="n" s="751">
-        <v>0.04260735337156643</v>
+        <v>0.04170113372407678</v>
       </c>
       <c r="I12" t="n" s="752">
-        <v>0.2762759715043035</v>
+        <v>0.263541834526379</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="740">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B13" t="n" s="745">
-        <v>0.7835337731239981</v>
+        <v>0.7450179533213644</v>
       </c>
       <c r="C13" t="n" s="746">
-        <v>0.7998792375094448</v>
+        <v>0.7875950609876448</v>
       </c>
       <c r="D13" t="n" s="747">
-        <v>0.8873814656462907</v>
+        <v>0.88031507063778</v>
       </c>
       <c r="E13" t="n" s="748">
-        <v>0.3075315889479226</v>
+        <v>0.2917840589756469</v>
       </c>
       <c r="F13" t="n" s="749">
-        <v>3.996982759583456</v>
+        <v>3.7079884519155732</v>
       </c>
       <c r="G13" t="n" s="750">
-        <v>0.030364285251343996</v>
+        <v>0.03434515220432574</v>
       </c>
       <c r="H13" t="n" s="751">
-        <v>0.0390192064594092</v>
+        <v>0.04241676751781244</v>
       </c>
       <c r="I13" t="n" s="752">
-        <v>0.2756190182154815</v>
+        <v>0.2721131085806219</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="740">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" t="n" s="745">
-        <v>0.7939072624758059</v>
+        <v>0.8019453976271439</v>
       </c>
       <c r="C14" t="n" s="746">
-        <v>0.8154515863523149</v>
+        <v>0.829742228715173</v>
       </c>
       <c r="D14" t="n" s="747">
-        <v>0.9011479018888681</v>
+        <v>0.9091927524113534</v>
       </c>
       <c r="E14" t="n" s="748">
-        <v>0.3292908113884034</v>
+        <v>0.3512787424292483</v>
       </c>
       <c r="F14" t="n" s="749">
-        <v>4.418632326523623</v>
+        <v>4.873447023613882</v>
       </c>
       <c r="G14" t="n" s="750">
-        <v>0.02885538679877749</v>
+        <v>0.026794288674363405</v>
       </c>
       <c r="H14" t="n" s="751">
-        <v>0.037465105171912705</v>
+        <v>0.05347927709939156</v>
       </c>
       <c r="I14" t="n" s="752">
-        <v>0.2792322916184503</v>
+        <v>0.28535253635633073</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="740">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B15" t="n" s="745">
-        <v>0.7741890270038578</v>
+        <v>0.7801832346557503</v>
       </c>
       <c r="C15" t="n" s="746">
-        <v>0.8076499416866227</v>
+        <v>0.8006499599531587</v>
       </c>
       <c r="D15" t="n" s="747">
-        <v>0.8859810534202965</v>
+        <v>0.8947383943957988</v>
       </c>
       <c r="E15" t="n" s="748">
-        <v>0.31812265372623755</v>
+        <v>0.3085593730146958</v>
       </c>
       <c r="F15" t="n" s="749">
-        <v>4.198854675524958</v>
+        <v>4.016301976989971</v>
       </c>
       <c r="G15" t="n" s="750">
-        <v>0.031583092654620226</v>
+        <v>0.0281608835257861</v>
       </c>
       <c r="H15" t="n" s="751">
-        <v>0.03951926433426033</v>
+        <v>0.06555032034605078</v>
       </c>
       <c r="I15" t="n" s="752">
-        <v>0.2756190182154815</v>
+        <v>0.24262460000121494</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="740">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B16" t="n" s="745">
-        <v>0.7764955802583744</v>
+        <v>0.7873586333968968</v>
       </c>
       <c r="C16" t="n" s="746">
-        <v>0.8069658002860638</v>
+        <v>0.8094280842661364</v>
       </c>
       <c r="D16" t="n" s="747">
-        <v>0.885900322925282</v>
+        <v>0.9007135734967451</v>
       </c>
       <c r="E16" t="n" s="748">
-        <v>0.31716942745933824</v>
+        <v>0.32061950220752716</v>
       </c>
       <c r="F16" t="n" s="749">
-        <v>4.1804291751510005</v>
+        <v>4.2473628978811035</v>
       </c>
       <c r="G16" t="n" s="750">
-        <v>0.03095744376961498</v>
+        <v>0.02697081907381177</v>
       </c>
       <c r="H16" t="n" s="751">
-        <v>0.04062827761010469</v>
+        <v>0.06440795179118408</v>
       </c>
       <c r="I16" t="n" s="752">
-        <v>0.279066446686835</v>
+        <v>0.2762759715043035</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="740">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B17" t="n" s="745">
-        <v>0.7560545497296025</v>
+        <v>0.7798258975051093</v>
       </c>
       <c r="C17" t="n" s="746">
-        <v>0.8014535441582366</v>
+        <v>0.8105881982695138</v>
       </c>
       <c r="D17" t="n" s="747">
-        <v>0.8665948843528842</v>
+        <v>0.8999396299554203</v>
       </c>
       <c r="E17" t="n" s="748">
-        <v>0.30963619353869637</v>
+        <v>0.32226374527297086</v>
       </c>
       <c r="F17" t="n" s="749">
-        <v>4.036604636231708</v>
+        <v>4.279502073597814</v>
       </c>
       <c r="G17" t="n" s="750">
-        <v>0.03592509269818063</v>
+        <v>0.026632263625435103</v>
       </c>
       <c r="H17" t="n" s="751">
-        <v>0.03490382656067487</v>
+        <v>0.06472738136548721</v>
       </c>
       <c r="I17" t="n" s="752">
-        <v>0.2762759715043035</v>
+        <v>0.2757848631470968</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="740">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B18" t="n" s="745">
-        <v>0.7579691798572625</v>
+        <v>0.7796440261865794</v>
       </c>
       <c r="C18" t="n" s="746">
-        <v>0.8004289105023551</v>
+        <v>0.8078273836692489</v>
       </c>
       <c r="D18" t="n" s="747">
-        <v>0.8665525014598444</v>
+        <v>0.8946782281637531</v>
       </c>
       <c r="E18" t="n" s="748">
-        <v>0.30826409698920637</v>
+        <v>0.31837055836294115</v>
       </c>
       <c r="F18" t="n" s="749">
-        <v>4.010745807507358</v>
+        <v>4.203655021685741</v>
       </c>
       <c r="G18" t="n" s="750">
-        <v>0.035727870057462786</v>
+        <v>0.026237375954719734</v>
       </c>
       <c r="H18" t="n" s="751">
-        <v>0.03535635863460925</v>
+        <v>0.06378992986449394</v>
       </c>
       <c r="I18" t="n" s="752">
-        <v>0.2756190182154815</v>
+        <v>0.2721131085806219</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="740">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B19" t="n" s="745">
-        <v>0.7841450404406292</v>
+        <v>0.7700844155844155</v>
       </c>
       <c r="C19" t="n" s="746">
-        <v>0.8132346759308386</v>
+        <v>0.8070408290112677</v>
       </c>
       <c r="D19" t="n" s="747">
-        <v>0.9026369684731685</v>
+        <v>0.8818758979144758</v>
       </c>
       <c r="E19" t="n" s="748">
-        <v>0.32606042636353005</v>
+        <v>0.31727376603955043</v>
       </c>
       <c r="F19" t="n" s="749">
-        <v>4.3543129860106635</v>
+        <v>4.1824434924546505</v>
       </c>
       <c r="G19" t="n" s="750">
-        <v>0.029876140777608803</v>
+        <v>0.02869919716420474</v>
       </c>
       <c r="H19" t="n" s="751">
-        <v>0.04325579936055766</v>
+        <v>0.05817733093143355</v>
       </c>
       <c r="I19" t="n" s="752">
-        <v>0.2792322916184503</v>
+        <v>0.2600359248915194</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="740">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B20" t="n" s="745">
-        <v>0.7805578436756362</v>
+        <v>0.7741344758167455</v>
       </c>
       <c r="C20" t="n" s="746">
-        <v>0.8072172813779488</v>
+        <v>0.8098471607943044</v>
       </c>
       <c r="D20" t="n" s="747">
-        <v>0.8958106026928925</v>
+        <v>0.8837908400368202</v>
       </c>
       <c r="E20" t="n" s="748">
-        <v>0.3175193434361975</v>
+        <v>0.32121206762543597</v>
       </c>
       <c r="F20" t="n" s="749">
-        <v>4.187186938474972</v>
+        <v>4.258927524706911</v>
       </c>
       <c r="G20" t="n" s="750">
-        <v>0.029725935496477448</v>
+        <v>0.027886514205116616</v>
       </c>
       <c r="H20" t="n" s="751">
-        <v>0.04442346020988523</v>
+        <v>0.05767840958462669</v>
       </c>
       <c r="I20" t="n" s="752">
-        <v>0.2756190182154815</v>
+        <v>0.2726042169378285</v>
       </c>
     </row>
     <row r="21">
@@ -7706,25 +7874,25 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="756">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="s" s="770">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s" s="770">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s" s="770">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s" s="770">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s" s="770">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G24" t="s" s="770">
         <v>9</v>
@@ -7735,262 +7903,262 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="766">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B25" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C25" t="n" s="772">
-        <v>0.6215645515597179</v>
+        <v>0.7823489285452881</v>
       </c>
       <c r="D25" t="n" s="773">
-        <v>0.7119481043272704</v>
+        <v>0.7094046861060817</v>
       </c>
       <c r="E25" t="n" s="774">
-        <v>0.68930633270788</v>
+        <v>0.7377732350447129</v>
       </c>
       <c r="F25" t="n" s="775">
-        <v>0.5554118787952328</v>
+        <v>0.7566876850612223</v>
       </c>
       <c r="G25" t="n" s="776">
-        <v>3.888888888888889</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="H25" t="n" s="777">
-        <v>0.8316309141225229</v>
+        <v>0.5023137559951615</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="766">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B26" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C26" t="n" s="772">
-        <v>0.537716785499387</v>
+        <v>0.8311398965494092</v>
       </c>
       <c r="D26" t="n" s="773">
-        <v>0.6524619724143322</v>
+        <v>0.7546718785448969</v>
       </c>
       <c r="E26" t="n" s="774">
-        <v>0.6018201893792149</v>
+        <v>0.7881676276247925</v>
       </c>
       <c r="F26" t="n" s="775">
-        <v>0.4546701632491625</v>
+        <v>0.7118020146765954</v>
       </c>
       <c r="G26" t="n" s="776">
-        <v>4.474747474747475</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="H26" t="n" s="777">
-        <v>0.9073783085152335</v>
+        <v>2.1869913932980913</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="766">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B27" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C27" t="n" s="772">
-        <v>0.5422525334442239</v>
+        <v>0.8260970490079553</v>
       </c>
       <c r="D27" t="n" s="773">
-        <v>0.655958563319035</v>
+        <v>0.7481424299199357</v>
       </c>
       <c r="E27" t="n" s="774">
-        <v>0.6293459396389934</v>
+        <v>0.776964974142428</v>
       </c>
       <c r="F27" t="n" s="775">
-        <v>0.47033208965995266</v>
+        <v>0.6978094183911678</v>
       </c>
       <c r="G27" t="n" s="776">
-        <v>3.9292929292929295</v>
+        <v>2.212121212121212</v>
       </c>
       <c r="H27" t="n" s="777">
-        <v>0.7986279720912847</v>
+        <v>2.264512053909309</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="766">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B28" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C28" t="n" s="772">
-        <v>0.39905929862179607</v>
+        <v>0.21346560159089453</v>
       </c>
       <c r="D28" t="n" s="773">
-        <v>0.5293124580217259</v>
+        <v>0.40189666888535286</v>
       </c>
       <c r="E28" t="n" s="774">
-        <v>0.4719540072471466</v>
+        <v>0.3135972033036981</v>
       </c>
       <c r="F28" t="n" s="775">
-        <v>0.3019285634583139</v>
+        <v>0.20168205096402203</v>
       </c>
       <c r="G28" t="n" s="776">
-        <v>4.515151515151516</v>
+        <v>0.98989898989899</v>
       </c>
       <c r="H28" t="n" s="777">
-        <v>0.9187795405622853</v>
+        <v>0.10050378152592121</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="766">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B29" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C29" t="n" s="772">
-        <v>0.6121414274806759</v>
+        <v>0.5480288539149466</v>
       </c>
       <c r="D29" t="n" s="773">
-        <v>0.5943149494999257</v>
+        <v>0.6505138513835955</v>
       </c>
       <c r="E29" t="n" s="774">
-        <v>0.5666879928088081</v>
+        <v>0.598777362802163</v>
       </c>
       <c r="F29" t="n" s="775">
-        <v>0.5063231313819051</v>
+        <v>0.47071328949392627</v>
       </c>
       <c r="G29" t="n" s="776">
-        <v>2.7373737373737375</v>
+        <v>3.888888888888889</v>
       </c>
       <c r="H29" t="n" s="777">
-        <v>1.2501906677918566</v>
+        <v>0.8316309141225229</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="766">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B30" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C30" t="n" s="772">
-        <v>0.5925857742171144</v>
+        <v>0.4547414292232948</v>
       </c>
       <c r="D30" t="n" s="773">
-        <v>0.5998630518965121</v>
+        <v>0.5803265948398432</v>
       </c>
       <c r="E30" t="n" s="774">
-        <v>0.5712880858006191</v>
+        <v>0.5121254298837264</v>
       </c>
       <c r="F30" t="n" s="775">
-        <v>0.48740975521616253</v>
+        <v>0.3600373845075743</v>
       </c>
       <c r="G30" t="n" s="776">
-        <v>2.3737373737373737</v>
+        <v>4.474747474747475</v>
       </c>
       <c r="H30" t="n" s="777">
-        <v>1.208691809150421</v>
+        <v>0.9073783085152335</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="766">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B31" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C31" t="n" s="772">
-        <v>0.7823632780567502</v>
+        <v>0.5975892237517714</v>
       </c>
       <c r="D31" t="n" s="773">
-        <v>0.6437090458860744</v>
+        <v>0.5707574676763311</v>
       </c>
       <c r="E31" t="n" s="774">
-        <v>0.6665049280815095</v>
+        <v>0.49877103646508214</v>
       </c>
       <c r="F31" t="n" s="775">
-        <v>0.6435847280360144</v>
+        <v>0.44371521057068364</v>
       </c>
       <c r="G31" t="n" s="776">
-        <v>2.1818181818181817</v>
+        <v>2.080808080808081</v>
       </c>
       <c r="H31" t="n" s="777">
-        <v>2.1869913932980913</v>
+        <v>1.6392928271041933</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="766">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B32" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C32" t="n" s="772">
-        <v>0.7857633025720442</v>
+        <v>0.5550548549731169</v>
       </c>
       <c r="D32" t="n" s="773">
-        <v>0.6516951163699858</v>
+        <v>0.5934149453913676</v>
       </c>
       <c r="E32" t="n" s="774">
-        <v>0.6748051760210102</v>
+        <v>0.5361373612194281</v>
       </c>
       <c r="F32" t="n" s="775">
-        <v>0.6420175359056941</v>
+        <v>0.429815922594027</v>
       </c>
       <c r="G32" t="n" s="776">
-        <v>2.212121212121212</v>
+        <v>2.727272727272727</v>
       </c>
       <c r="H32" t="n" s="777">
-        <v>2.264512053909309</v>
+        <v>1.3000642199065635</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="766">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B33" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C33" t="n" s="772">
-        <v>0.5779162057307503</v>
+        <v>0.6259555962348334</v>
       </c>
       <c r="D33" t="n" s="773">
-        <v>0.5481144020309864</v>
+        <v>0.5997980315877244</v>
       </c>
       <c r="E33" t="n" s="774">
-        <v>0.47826098268108547</v>
+        <v>0.5754650000201859</v>
       </c>
       <c r="F33" t="n" s="775">
-        <v>0.4257950899388788</v>
+        <v>0.51856698078874</v>
       </c>
       <c r="G33" t="n" s="776">
-        <v>2.080808080808081</v>
+        <v>2.7373737373737375</v>
       </c>
       <c r="H33" t="n" s="777">
-        <v>1.6392928271041933</v>
+        <v>1.2501906677918566</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="766">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B34" t="n" s="771">
         <v>99.0</v>
       </c>
       <c r="C34" t="n" s="772">
-        <v>0.5627794317407216</v>
+        <v>0.5932582659231942</v>
       </c>
       <c r="D34" t="n" s="773">
-        <v>0.5978264214161838</v>
+        <v>0.5768779965420368</v>
       </c>
       <c r="E34" t="n" s="774">
-        <v>0.5440489686615094</v>
+        <v>0.5488086167222136</v>
       </c>
       <c r="F34" t="n" s="775">
-        <v>0.44349896446244513</v>
+        <v>0.4840841706562902</v>
       </c>
       <c r="G34" t="n" s="776">
-        <v>2.727272727272727</v>
+        <v>2.3737373737373737</v>
       </c>
       <c r="H34" t="n" s="777">
-        <v>1.3000642199065635</v>
+        <v>1.208691809150421</v>
       </c>
     </row>
     <row r="35">
@@ -8005,54 +8173,54 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="781">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38">
       <c r="A38"/>
       <c r="B38" t="s" s="795">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s" s="795">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s" s="795">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E38" t="s" s="795">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F38" t="s" s="795">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G38" t="s" s="795">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H38" t="s" s="795">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="791">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B39" t="n" s="796">
-        <v>0.010101010101010102</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="C39" t="n" s="797">
-        <v>0.010101010101010102</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="D39" t="n" s="798">
         <v>0.0</v>
       </c>
       <c r="E39" t="n" s="799">
-        <v>0.24242424242424243</v>
+        <v>0.0</v>
       </c>
       <c r="F39" t="n" s="800">
-        <v>0.5353535353535354</v>
+        <v>0.0</v>
       </c>
       <c r="G39" t="n" s="801">
-        <v>0.20202020202020202</v>
+        <v>0.0</v>
       </c>
       <c r="H39" t="n" s="802">
         <v>0.0</v>
@@ -8060,10 +8228,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="791">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B40" t="n" s="796">
-        <v>0.010101010101010102</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="C40" t="n" s="797">
         <v>0.0</v>
@@ -8072,13 +8240,13 @@
         <v>0.0</v>
       </c>
       <c r="E40" t="n" s="799">
-        <v>0.18181818181818182</v>
+        <v>0.08080808080808081</v>
       </c>
       <c r="F40" t="n" s="800">
-        <v>0.1111111111111111</v>
+        <v>0.23232323232323232</v>
       </c>
       <c r="G40" t="n" s="801">
-        <v>0.696969696969697</v>
+        <v>0.20202020202020202</v>
       </c>
       <c r="H40" t="n" s="802">
         <v>0.0</v>
@@ -8086,25 +8254,25 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="791">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B41" t="n" s="796">
-        <v>0.0</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="C41" t="n" s="797">
-        <v>0.020202020202020204</v>
+        <v>0.0</v>
       </c>
       <c r="D41" t="n" s="798">
-        <v>0.010101010101010102</v>
+        <v>0.030303030303030304</v>
       </c>
       <c r="E41" t="n" s="799">
-        <v>0.20202020202020202</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="F41" t="n" s="800">
-        <v>0.5555555555555556</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="G41" t="n" s="801">
-        <v>0.21212121212121213</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="H41" t="n" s="802">
         <v>0.0</v>
@@ -8112,25 +8280,25 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="791">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B42" t="n" s="796">
-        <v>0.0</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="C42" t="n" s="797">
-        <v>0.010101010101010102</v>
+        <v>0.98989898989899</v>
       </c>
       <c r="D42" t="n" s="798">
-        <v>0.020202020202020204</v>
+        <v>0.0</v>
       </c>
       <c r="E42" t="n" s="799">
-        <v>0.1717171717171717</v>
+        <v>0.0</v>
       </c>
       <c r="F42" t="n" s="800">
-        <v>0.04040404040404041</v>
+        <v>0.0</v>
       </c>
       <c r="G42" t="n" s="801">
-        <v>0.7575757575757576</v>
+        <v>0.0</v>
       </c>
       <c r="H42" t="n" s="802">
         <v>0.0</v>
@@ -8138,25 +8306,25 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="791">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B43" t="n" s="796">
-        <v>0.10101010101010101</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="C43" t="n" s="797">
         <v>0.010101010101010102</v>
       </c>
       <c r="D43" t="n" s="798">
-        <v>0.30303030303030304</v>
+        <v>0.0</v>
       </c>
       <c r="E43" t="n" s="799">
-        <v>0.2222222222222222</v>
+        <v>0.24242424242424243</v>
       </c>
       <c r="F43" t="n" s="800">
-        <v>0.36363636363636365</v>
+        <v>0.5353535353535354</v>
       </c>
       <c r="G43" t="n" s="801">
-        <v>0.0</v>
+        <v>0.20202020202020202</v>
       </c>
       <c r="H43" t="n" s="802">
         <v>0.0</v>
@@ -8164,25 +8332,25 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="791">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B44" t="n" s="796">
-        <v>0.13131313131313133</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="C44" t="n" s="797">
-        <v>0.010101010101010102</v>
+        <v>0.0</v>
       </c>
       <c r="D44" t="n" s="798">
-        <v>0.41414141414141414</v>
+        <v>0.0</v>
       </c>
       <c r="E44" t="n" s="799">
-        <v>0.24242424242424243</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="F44" t="n" s="800">
-        <v>0.20202020202020202</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G44" t="n" s="801">
-        <v>0.0</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="H44" t="n" s="802">
         <v>0.0</v>
@@ -8190,25 +8358,25 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="791">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B45" t="n" s="796">
-        <v>0.48484848484848486</v>
+        <v>0.32323232323232326</v>
       </c>
       <c r="C45" t="n" s="797">
-        <v>0.0</v>
+        <v>0.06060606060606061</v>
       </c>
       <c r="D45" t="n" s="798">
-        <v>0.0</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="E45" t="n" s="799">
-        <v>0.08080808080808081</v>
+        <v>0.26262626262626265</v>
       </c>
       <c r="F45" t="n" s="800">
-        <v>0.23232323232323232</v>
+        <v>0.26262626262626265</v>
       </c>
       <c r="G45" t="n" s="801">
-        <v>0.20202020202020202</v>
+        <v>0.0</v>
       </c>
       <c r="H45" t="n" s="802">
         <v>0.0</v>
@@ -8216,25 +8384,25 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="791">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B46" t="n" s="796">
-        <v>0.48484848484848486</v>
+        <v>0.1414141414141414</v>
       </c>
       <c r="C46" t="n" s="797">
-        <v>0.0</v>
+        <v>0.030303030303030304</v>
       </c>
       <c r="D46" t="n" s="798">
-        <v>0.030303030303030304</v>
+        <v>0.0707070707070707</v>
       </c>
       <c r="E46" t="n" s="799">
-        <v>0.09090909090909091</v>
+        <v>0.47474747474747475</v>
       </c>
       <c r="F46" t="n" s="800">
-        <v>0.09090909090909091</v>
+        <v>0.2828282828282828</v>
       </c>
       <c r="G46" t="n" s="801">
-        <v>0.30303030303030304</v>
+        <v>0.0</v>
       </c>
       <c r="H46" t="n" s="802">
         <v>0.0</v>
@@ -8242,22 +8410,22 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="791">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B47" t="n" s="796">
-        <v>0.32323232323232326</v>
+        <v>0.10101010101010101</v>
       </c>
       <c r="C47" t="n" s="797">
-        <v>0.06060606060606061</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="D47" t="n" s="798">
-        <v>0.09090909090909091</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="E47" t="n" s="799">
-        <v>0.26262626262626265</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="F47" t="n" s="800">
-        <v>0.26262626262626265</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="G47" t="n" s="801">
         <v>0.0</v>
@@ -8268,22 +8436,22 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="791">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B48" t="n" s="796">
-        <v>0.1414141414141414</v>
+        <v>0.13131313131313133</v>
       </c>
       <c r="C48" t="n" s="797">
-        <v>0.030303030303030304</v>
+        <v>0.010101010101010102</v>
       </c>
       <c r="D48" t="n" s="798">
-        <v>0.0707070707070707</v>
+        <v>0.41414141414141414</v>
       </c>
       <c r="E48" t="n" s="799">
-        <v>0.47474747474747475</v>
+        <v>0.24242424242424243</v>
       </c>
       <c r="F48" t="n" s="800">
-        <v>0.2828282828282828</v>
+        <v>0.20202020202020202</v>
       </c>
       <c r="G48" t="n" s="801">
         <v>0.0</v>

</xml_diff>